<commit_message>
Add data for 2023-07-01
</commit_message>
<xml_diff>
--- a/output/cta-index-crime-ytd.xlsx
+++ b/output/cta-index-crime-ytd.xlsx
@@ -36,28 +36,28 @@
     <sheet name="New City" sheetId="27" r:id="rId27"/>
     <sheet name="Lake View" sheetId="28" r:id="rId28"/>
     <sheet name="Washington Heights" sheetId="29" r:id="rId29"/>
-    <sheet name="West Loop" sheetId="30" r:id="rId30"/>
+    <sheet name="North Lawndale" sheetId="30" r:id="rId30"/>
     <sheet name="Sheffield &amp; DePaul" sheetId="31" r:id="rId31"/>
     <sheet name="West Pullman" sheetId="32" r:id="rId32"/>
     <sheet name="North Center" sheetId="33" r:id="rId33"/>
     <sheet name="Norwood Park" sheetId="34" r:id="rId34"/>
     <sheet name="Wrigleyville" sheetId="35" r:id="rId35"/>
     <sheet name="Bucktown" sheetId="36" r:id="rId36"/>
-    <sheet name="Rogers Park" sheetId="37" r:id="rId37"/>
-    <sheet name="Roseland" sheetId="38" r:id="rId38"/>
-    <sheet name="West Lawn" sheetId="39" r:id="rId39"/>
-    <sheet name="Austin" sheetId="40" r:id="rId40"/>
-    <sheet name="Wicker Park" sheetId="41" r:id="rId41"/>
-    <sheet name="Ukrainian Village" sheetId="42" r:id="rId42"/>
-    <sheet name="Little Italy, UIC" sheetId="43" r:id="rId43"/>
-    <sheet name="Archer Heights" sheetId="44" r:id="rId44"/>
-    <sheet name="Bridgeport" sheetId="45" r:id="rId45"/>
-    <sheet name="Montclare" sheetId="46" r:id="rId46"/>
-    <sheet name="Old Town" sheetId="47" r:id="rId47"/>
-    <sheet name="O'Hare" sheetId="48" r:id="rId48"/>
-    <sheet name="Grant Park" sheetId="49" r:id="rId49"/>
-    <sheet name="Lincoln Park" sheetId="50" r:id="rId50"/>
-    <sheet name="North Lawndale" sheetId="51" r:id="rId51"/>
+    <sheet name="West Loop" sheetId="37" r:id="rId37"/>
+    <sheet name="Rogers Park" sheetId="38" r:id="rId38"/>
+    <sheet name="Roseland" sheetId="39" r:id="rId39"/>
+    <sheet name="West Lawn" sheetId="40" r:id="rId40"/>
+    <sheet name="Austin" sheetId="41" r:id="rId41"/>
+    <sheet name="Wicker Park" sheetId="42" r:id="rId42"/>
+    <sheet name="Ukrainian Village" sheetId="43" r:id="rId43"/>
+    <sheet name="Little Italy, UIC" sheetId="44" r:id="rId44"/>
+    <sheet name="Archer Heights" sheetId="45" r:id="rId45"/>
+    <sheet name="Bridgeport" sheetId="46" r:id="rId46"/>
+    <sheet name="Montclare" sheetId="47" r:id="rId47"/>
+    <sheet name="Old Town" sheetId="48" r:id="rId48"/>
+    <sheet name="O'Hare" sheetId="49" r:id="rId49"/>
+    <sheet name="Grant Park" sheetId="50" r:id="rId50"/>
+    <sheet name="Lincoln Park" sheetId="51" r:id="rId51"/>
     <sheet name="Auburn Gresham" sheetId="52" r:id="rId52"/>
     <sheet name="Brighton Park" sheetId="53" r:id="rId53"/>
     <sheet name="Logan Square" sheetId="54" r:id="rId54"/>
@@ -7937,7 +7937,7 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7991,7 +7991,13 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
         <v>1</v>
       </c>
       <c r="G2">
@@ -8008,134 +8014,141 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3">
-        <v>2</v>
+      <c r="C3">
+        <v>1</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
       <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
         <v>1</v>
       </c>
       <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="I4">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5">
+        <v>5</v>
+      </c>
+      <c r="H5">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6">
         <v>7</v>
       </c>
       <c r="D6">
+        <v>12</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>14</v>
+      </c>
+      <c r="G6">
+        <v>8</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="I6">
+        <v>11</v>
+      </c>
+      <c r="J6">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>12</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="E7">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="G7">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="H7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I7">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J7">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C8">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D8">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="E8">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F8">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="G8">
+        <v>30</v>
+      </c>
+      <c r="H8">
         <v>12</v>
       </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
       <c r="I8">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>14</v>
-      </c>
-      <c r="C9">
-        <v>7</v>
-      </c>
-      <c r="D9">
-        <v>22</v>
-      </c>
-      <c r="E9">
-        <v>19</v>
-      </c>
-      <c r="F9">
-        <v>28</v>
-      </c>
-      <c r="G9">
-        <v>18</v>
-      </c>
-      <c r="H9">
-        <v>8</v>
-      </c>
-      <c r="I9">
-        <v>21</v>
-      </c>
-      <c r="J9">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -9119,6 +9132,214 @@
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>16</v>
+      </c>
+      <c r="E8">
+        <v>15</v>
+      </c>
+      <c r="F8">
+        <v>25</v>
+      </c>
+      <c r="G8">
+        <v>12</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>15</v>
+      </c>
+      <c r="J8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>14</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>22</v>
+      </c>
+      <c r="E9">
+        <v>19</v>
+      </c>
+      <c r="F9">
+        <v>28</v>
+      </c>
+      <c r="G9">
+        <v>18</v>
+      </c>
+      <c r="H9">
+        <v>8</v>
+      </c>
+      <c r="I9">
+        <v>21</v>
+      </c>
+      <c r="J9">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9329,7 +9550,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J9"/>
   <sheetViews>
@@ -9551,110 +9772,6 @@
       </c>
       <c r="J9">
         <v>35</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="E5">
-        <v>3</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -9845,6 +9962,110 @@
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -10085,7 +10306,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -10248,7 +10469,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -10347,7 +10568,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J7"/>
   <sheetViews>
@@ -10545,7 +10766,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F6"/>
   <sheetViews>
@@ -10644,7 +10865,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J5"/>
   <sheetViews>
@@ -10799,7 +11020,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -10875,7 +11096,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J7"/>
   <sheetViews>
@@ -11076,7 +11297,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -11229,92 +11450,6 @@
       </c>
       <c r="J6">
         <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -11580,6 +11715,92 @@
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -11735,227 +11956,6 @@
       </c>
       <c r="I7">
         <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>3</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>6</v>
-      </c>
-      <c r="C6">
-        <v>7</v>
-      </c>
-      <c r="D6">
-        <v>12</v>
-      </c>
-      <c r="E6">
-        <v>4</v>
-      </c>
-      <c r="F6">
-        <v>14</v>
-      </c>
-      <c r="G6">
-        <v>8</v>
-      </c>
-      <c r="H6">
-        <v>5</v>
-      </c>
-      <c r="I6">
-        <v>11</v>
-      </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>11</v>
-      </c>
-      <c r="C7">
-        <v>12</v>
-      </c>
-      <c r="D7">
-        <v>16</v>
-      </c>
-      <c r="E7">
-        <v>12</v>
-      </c>
-      <c r="F7">
-        <v>17</v>
-      </c>
-      <c r="G7">
-        <v>19</v>
-      </c>
-      <c r="H7">
-        <v>2</v>
-      </c>
-      <c r="I7">
-        <v>6</v>
-      </c>
-      <c r="J7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8">
-        <v>18</v>
-      </c>
-      <c r="C8">
-        <v>20</v>
-      </c>
-      <c r="D8">
-        <v>29</v>
-      </c>
-      <c r="E8">
-        <v>18</v>
-      </c>
-      <c r="F8">
-        <v>33</v>
-      </c>
-      <c r="G8">
-        <v>30</v>
-      </c>
-      <c r="H8">
-        <v>12</v>
-      </c>
-      <c r="I8">
-        <v>20</v>
-      </c>
-      <c r="J8">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2023-07-02
</commit_message>
<xml_diff>
--- a/output/cta-index-crime-ytd.xlsx
+++ b/output/cta-index-crime-ytd.xlsx
@@ -36,28 +36,28 @@
     <sheet name="New City" sheetId="27" r:id="rId27"/>
     <sheet name="Lake View" sheetId="28" r:id="rId28"/>
     <sheet name="Washington Heights" sheetId="29" r:id="rId29"/>
-    <sheet name="West Loop" sheetId="30" r:id="rId30"/>
+    <sheet name="North Lawndale" sheetId="30" r:id="rId30"/>
     <sheet name="Sheffield &amp; DePaul" sheetId="31" r:id="rId31"/>
     <sheet name="West Pullman" sheetId="32" r:id="rId32"/>
     <sheet name="North Center" sheetId="33" r:id="rId33"/>
     <sheet name="Norwood Park" sheetId="34" r:id="rId34"/>
     <sheet name="Wrigleyville" sheetId="35" r:id="rId35"/>
     <sheet name="Bucktown" sheetId="36" r:id="rId36"/>
-    <sheet name="Rogers Park" sheetId="37" r:id="rId37"/>
-    <sheet name="Roseland" sheetId="38" r:id="rId38"/>
-    <sheet name="West Lawn" sheetId="39" r:id="rId39"/>
-    <sheet name="Austin" sheetId="40" r:id="rId40"/>
-    <sheet name="Wicker Park" sheetId="41" r:id="rId41"/>
-    <sheet name="Ukrainian Village" sheetId="42" r:id="rId42"/>
-    <sheet name="Little Italy, UIC" sheetId="43" r:id="rId43"/>
-    <sheet name="Archer Heights" sheetId="44" r:id="rId44"/>
-    <sheet name="Bridgeport" sheetId="45" r:id="rId45"/>
-    <sheet name="Montclare" sheetId="46" r:id="rId46"/>
-    <sheet name="Old Town" sheetId="47" r:id="rId47"/>
-    <sheet name="O'Hare" sheetId="48" r:id="rId48"/>
-    <sheet name="Grant Park" sheetId="49" r:id="rId49"/>
-    <sheet name="Lincoln Park" sheetId="50" r:id="rId50"/>
-    <sheet name="North Lawndale" sheetId="51" r:id="rId51"/>
+    <sheet name="West Loop" sheetId="37" r:id="rId37"/>
+    <sheet name="Rogers Park" sheetId="38" r:id="rId38"/>
+    <sheet name="Roseland" sheetId="39" r:id="rId39"/>
+    <sheet name="West Lawn" sheetId="40" r:id="rId40"/>
+    <sheet name="Austin" sheetId="41" r:id="rId41"/>
+    <sheet name="Wicker Park" sheetId="42" r:id="rId42"/>
+    <sheet name="Ukrainian Village" sheetId="43" r:id="rId43"/>
+    <sheet name="Little Italy, UIC" sheetId="44" r:id="rId44"/>
+    <sheet name="Archer Heights" sheetId="45" r:id="rId45"/>
+    <sheet name="Bridgeport" sheetId="46" r:id="rId46"/>
+    <sheet name="Montclare" sheetId="47" r:id="rId47"/>
+    <sheet name="Old Town" sheetId="48" r:id="rId48"/>
+    <sheet name="O'Hare" sheetId="49" r:id="rId49"/>
+    <sheet name="Grant Park" sheetId="50" r:id="rId50"/>
+    <sheet name="Lincoln Park" sheetId="51" r:id="rId51"/>
     <sheet name="Auburn Gresham" sheetId="52" r:id="rId52"/>
     <sheet name="Brighton Park" sheetId="53" r:id="rId53"/>
     <sheet name="Logan Square" sheetId="54" r:id="rId54"/>
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="108">
   <si>
     <t>crime_category</t>
   </si>
@@ -877,7 +877,7 @@
         <v>50</v>
       </c>
       <c r="H2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I2">
         <v>52</v>
@@ -900,10 +900,10 @@
         <v>72</v>
       </c>
       <c r="E3">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F3">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G3">
         <v>59</v>
@@ -991,6 +991,9 @@
       <c r="G7">
         <v>2</v>
       </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
       <c r="I7">
         <v>2</v>
       </c>
@@ -1023,7 +1026,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C9">
         <v>233</v>
@@ -1032,22 +1035,22 @@
         <v>221</v>
       </c>
       <c r="E9">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F9">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="G9">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="H9">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="I9">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="J9">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1055,28 +1058,28 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>561</v>
+        <v>566</v>
       </c>
       <c r="C10">
-        <v>687</v>
+        <v>690</v>
       </c>
       <c r="D10">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="E10">
-        <v>1053</v>
+        <v>1061</v>
       </c>
       <c r="F10">
-        <v>1123</v>
+        <v>1127</v>
       </c>
       <c r="G10">
-        <v>601</v>
+        <v>604</v>
       </c>
       <c r="H10">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="I10">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="J10">
         <v>380</v>
@@ -1087,31 +1090,31 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>813</v>
+        <v>819</v>
       </c>
       <c r="C11">
-        <v>1007</v>
+        <v>1010</v>
       </c>
       <c r="D11">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="E11">
-        <v>1390</v>
+        <v>1400</v>
       </c>
       <c r="F11">
-        <v>1492</v>
+        <v>1500</v>
       </c>
       <c r="G11">
-        <v>953</v>
+        <v>963</v>
       </c>
       <c r="H11">
-        <v>562</v>
+        <v>570</v>
       </c>
       <c r="I11">
-        <v>868</v>
+        <v>872</v>
       </c>
       <c r="J11">
-        <v>765</v>
+        <v>766</v>
       </c>
     </row>
   </sheetData>
@@ -1690,7 +1693,7 @@
         <v>17</v>
       </c>
       <c r="F7">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G7">
         <v>29</v>
@@ -1716,13 +1719,13 @@
         <v>27</v>
       </c>
       <c r="D8">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E8">
         <v>43</v>
       </c>
       <c r="F8">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G8">
         <v>35</v>
@@ -1748,13 +1751,13 @@
         <v>45</v>
       </c>
       <c r="D9">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E9">
         <v>68</v>
       </c>
       <c r="F9">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G9">
         <v>69</v>
@@ -1834,7 +1837,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -1956,7 +1959,7 @@
         <v>13</v>
       </c>
       <c r="H6">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I6">
         <v>18</v>
@@ -2102,13 +2105,13 @@
         <v>10</v>
       </c>
       <c r="E5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F5">
         <v>7</v>
       </c>
       <c r="G5">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H5">
         <v>4</v>
@@ -2134,13 +2137,13 @@
         <v>14</v>
       </c>
       <c r="E6">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F6">
         <v>9</v>
       </c>
       <c r="G6">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H6">
         <v>7</v>
@@ -2283,7 +2286,7 @@
         <v>1</v>
       </c>
       <c r="I5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J5">
         <v>7</v>
@@ -2294,7 +2297,7 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C6">
         <v>8</v>
@@ -2326,7 +2329,7 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7">
         <v>11</v>
@@ -2347,7 +2350,7 @@
         <v>5</v>
       </c>
       <c r="I7">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J7">
         <v>13</v>
@@ -2638,7 +2641,7 @@
         <v>2</v>
       </c>
       <c r="F5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G5">
         <v>3</v>
@@ -2670,7 +2673,7 @@
         <v>2</v>
       </c>
       <c r="F6">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G6">
         <v>6</v>
@@ -2841,7 +2844,7 @@
         <v>4</v>
       </c>
       <c r="J7">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -2905,7 +2908,7 @@
         <v>13</v>
       </c>
       <c r="J9">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -3048,7 +3051,7 @@
         <v>3</v>
       </c>
       <c r="I5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -3080,7 +3083,7 @@
         <v>3</v>
       </c>
       <c r="I6">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J6">
         <v>5</v>
@@ -3214,7 +3217,7 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5">
         <v>11</v>
@@ -3235,7 +3238,7 @@
         <v>5</v>
       </c>
       <c r="I5">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J5">
         <v>13</v>
@@ -3278,7 +3281,7 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C7">
         <v>20</v>
@@ -3287,7 +3290,7 @@
         <v>12</v>
       </c>
       <c r="E7">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F7">
         <v>11</v>
@@ -3296,7 +3299,7 @@
         <v>25</v>
       </c>
       <c r="H7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I7">
         <v>11</v>
@@ -3310,7 +3313,7 @@
         <v>18</v>
       </c>
       <c r="B8">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C8">
         <v>48</v>
@@ -3608,7 +3611,7 @@
         <v>21</v>
       </c>
       <c r="H19">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I19">
         <v>15</v>
@@ -3640,7 +3643,7 @@
         <v>8</v>
       </c>
       <c r="H20">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I20">
         <v>4</v>
@@ -3672,7 +3675,7 @@
         <v>5</v>
       </c>
       <c r="H21">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I21">
         <v>15</v>
@@ -3695,7 +3698,7 @@
         <v>8</v>
       </c>
       <c r="E22">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F22">
         <v>3</v>
@@ -3816,7 +3819,7 @@
         <v>15</v>
       </c>
       <c r="E27">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F27">
         <v>12</v>
@@ -3964,13 +3967,13 @@
         <v>45</v>
       </c>
       <c r="D32">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E32">
         <v>68</v>
       </c>
       <c r="F32">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G32">
         <v>69</v>
@@ -4010,7 +4013,7 @@
         <v>44</v>
       </c>
       <c r="E34">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I34">
         <v>1</v>
@@ -4065,16 +4068,16 @@
         <v>41</v>
       </c>
       <c r="E36">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F36">
         <v>42</v>
       </c>
       <c r="G36">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H36">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I36">
         <v>45</v>
@@ -4129,7 +4132,7 @@
         <v>4</v>
       </c>
       <c r="I38">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J38">
         <v>2</v>
@@ -4180,13 +4183,13 @@
         <v>14</v>
       </c>
       <c r="E41">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F41">
         <v>9</v>
       </c>
       <c r="G41">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H41">
         <v>7</v>
@@ -4250,7 +4253,7 @@
         <v>2</v>
       </c>
       <c r="G43">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H43">
         <v>2</v>
@@ -4328,7 +4331,7 @@
         <v>2</v>
       </c>
       <c r="F46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G46">
         <v>2</v>
@@ -4348,7 +4351,7 @@
         <v>57</v>
       </c>
       <c r="B47">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C47">
         <v>35</v>
@@ -4357,7 +4360,7 @@
         <v>30</v>
       </c>
       <c r="E47">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F47">
         <v>41</v>
@@ -4453,7 +4456,7 @@
         <v>22</v>
       </c>
       <c r="F50">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G50">
         <v>21</v>
@@ -4485,7 +4488,7 @@
         <v>2</v>
       </c>
       <c r="F51">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G51">
         <v>6</v>
@@ -4549,13 +4552,13 @@
         <v>356</v>
       </c>
       <c r="F53">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="G53">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="H53">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I53">
         <v>174</v>
@@ -4659,7 +4662,7 @@
         <v>2</v>
       </c>
       <c r="E57">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J57">
         <v>1</v>
@@ -4852,7 +4855,7 @@
         <v>18</v>
       </c>
       <c r="C65">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D65">
         <v>29</v>
@@ -4861,7 +4864,7 @@
         <v>18</v>
       </c>
       <c r="F65">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G65">
         <v>30</v>
@@ -4994,13 +4997,13 @@
         <v>28</v>
       </c>
       <c r="E70">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F70">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G70">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H70">
         <v>14</v>
@@ -5061,7 +5064,7 @@
         <v>23</v>
       </c>
       <c r="G72">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H72">
         <v>2</v>
@@ -5104,13 +5107,13 @@
         <v>54</v>
       </c>
       <c r="G74">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H74">
         <v>7</v>
       </c>
       <c r="I74">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J74">
         <v>21</v>
@@ -5147,7 +5150,7 @@
         <v>19</v>
       </c>
       <c r="C76">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D76">
         <v>27</v>
@@ -5176,7 +5179,7 @@
         <v>87</v>
       </c>
       <c r="B77">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C77">
         <v>36</v>
@@ -5226,7 +5229,7 @@
         <v>13</v>
       </c>
       <c r="H78">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I78">
         <v>18</v>
@@ -5255,7 +5258,7 @@
         <v>21</v>
       </c>
       <c r="G79">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H79">
         <v>6</v>
@@ -5467,7 +5470,7 @@
         <v>13</v>
       </c>
       <c r="J86">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="87" spans="1:10">
@@ -5528,7 +5531,7 @@
         <v>3</v>
       </c>
       <c r="I88">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J88">
         <v>5</v>
@@ -5641,7 +5644,7 @@
         <v>2</v>
       </c>
       <c r="H92">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I92">
         <v>2</v>
@@ -5658,7 +5661,7 @@
         <v>2</v>
       </c>
       <c r="C93">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D93">
         <v>2</v>
@@ -5809,31 +5812,31 @@
         <v>10</v>
       </c>
       <c r="B98">
-        <v>813</v>
+        <v>819</v>
       </c>
       <c r="C98">
-        <v>1007</v>
+        <v>1010</v>
       </c>
       <c r="D98">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="E98">
-        <v>1390</v>
+        <v>1400</v>
       </c>
       <c r="F98">
-        <v>1492</v>
+        <v>1500</v>
       </c>
       <c r="G98">
-        <v>953</v>
+        <v>963</v>
       </c>
       <c r="H98">
-        <v>562</v>
+        <v>570</v>
       </c>
       <c r="I98">
-        <v>868</v>
+        <v>872</v>
       </c>
       <c r="J98">
-        <v>765</v>
+        <v>766</v>
       </c>
     </row>
   </sheetData>
@@ -6440,7 +6443,7 @@
         <v>3</v>
       </c>
       <c r="H6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I6">
         <v>6</v>
@@ -6504,7 +6507,7 @@
         <v>5</v>
       </c>
       <c r="H8">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I8">
         <v>15</v>
@@ -6762,6 +6765,9 @@
       <c r="G4">
         <v>1</v>
       </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
@@ -6858,7 +6864,7 @@
         <v>21</v>
       </c>
       <c r="H8">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I8">
         <v>15</v>
@@ -7513,7 +7519,7 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7">
         <v>19</v>
@@ -7522,7 +7528,7 @@
         <v>24</v>
       </c>
       <c r="E7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F7">
         <v>32</v>
@@ -7545,7 +7551,7 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C8">
         <v>35</v>
@@ -7554,7 +7560,7 @@
         <v>30</v>
       </c>
       <c r="E8">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F8">
         <v>41</v>
@@ -7937,7 +7943,7 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7991,7 +7997,13 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
         <v>1</v>
       </c>
       <c r="G2">
@@ -8008,134 +8020,141 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3">
-        <v>2</v>
+      <c r="C3">
+        <v>1</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
       <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
         <v>1</v>
       </c>
       <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="I4">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5">
+        <v>5</v>
+      </c>
+      <c r="H5">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6">
         <v>7</v>
       </c>
       <c r="D6">
+        <v>12</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>14</v>
+      </c>
+      <c r="G6">
+        <v>8</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="I6">
+        <v>11</v>
+      </c>
+      <c r="J6">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>13</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="E7">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="G7">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="H7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I7">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J7">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C8">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="D8">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="E8">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F8">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="G8">
+        <v>30</v>
+      </c>
+      <c r="H8">
         <v>12</v>
       </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
       <c r="I8">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>14</v>
-      </c>
-      <c r="C9">
-        <v>7</v>
-      </c>
-      <c r="D9">
-        <v>22</v>
-      </c>
-      <c r="E9">
-        <v>19</v>
-      </c>
-      <c r="F9">
-        <v>28</v>
-      </c>
-      <c r="G9">
-        <v>18</v>
-      </c>
-      <c r="H9">
-        <v>8</v>
-      </c>
-      <c r="I9">
-        <v>21</v>
-      </c>
-      <c r="J9">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -8263,7 +8282,7 @@
         <v>4</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -8327,7 +8346,7 @@
         <v>21</v>
       </c>
       <c r="G7">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H7">
         <v>6</v>
@@ -8472,6 +8491,9 @@
       <c r="G5">
         <v>1</v>
       </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
@@ -8496,7 +8518,7 @@
         <v>2</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I6">
         <v>2</v>
@@ -9119,6 +9141,214 @@
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>16</v>
+      </c>
+      <c r="E8">
+        <v>15</v>
+      </c>
+      <c r="F8">
+        <v>25</v>
+      </c>
+      <c r="G8">
+        <v>12</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>15</v>
+      </c>
+      <c r="J8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>14</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>22</v>
+      </c>
+      <c r="E9">
+        <v>19</v>
+      </c>
+      <c r="F9">
+        <v>28</v>
+      </c>
+      <c r="G9">
+        <v>18</v>
+      </c>
+      <c r="H9">
+        <v>8</v>
+      </c>
+      <c r="I9">
+        <v>21</v>
+      </c>
+      <c r="J9">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9268,7 +9498,7 @@
         <v>18</v>
       </c>
       <c r="C7">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D7">
         <v>22</v>
@@ -9300,7 +9530,7 @@
         <v>19</v>
       </c>
       <c r="C8">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D8">
         <v>27</v>
@@ -9329,7 +9559,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J9"/>
   <sheetViews>
@@ -9494,7 +9724,7 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C8">
         <v>24</v>
@@ -9526,7 +9756,7 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C9">
         <v>36</v>
@@ -9551,110 +9781,6 @@
       </c>
       <c r="J9">
         <v>35</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="E5">
-        <v>3</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -9845,6 +9971,110 @@
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -10021,7 +10251,7 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7">
         <v>24</v>
@@ -10053,7 +10283,7 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C8">
         <v>48</v>
@@ -10085,7 +10315,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -10248,7 +10478,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -10347,7 +10577,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J7"/>
   <sheetViews>
@@ -10461,7 +10691,7 @@
         <v>9</v>
       </c>
       <c r="F5">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G5">
         <v>13</v>
@@ -10525,7 +10755,7 @@
         <v>22</v>
       </c>
       <c r="F7">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G7">
         <v>21</v>
@@ -10545,7 +10775,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F6"/>
   <sheetViews>
@@ -10644,7 +10874,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J5"/>
   <sheetViews>
@@ -10799,7 +11029,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -10875,7 +11105,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J7"/>
   <sheetViews>
@@ -10955,7 +11185,7 @@
         <v>1</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -10995,7 +11225,7 @@
         <v>11</v>
       </c>
       <c r="G5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H5">
         <v>6</v>
@@ -11021,7 +11251,7 @@
         <v>22</v>
       </c>
       <c r="E6">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F6">
         <v>61</v>
@@ -11053,13 +11283,13 @@
         <v>28</v>
       </c>
       <c r="E7">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F7">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G7">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H7">
         <v>14</v>
@@ -11076,7 +11306,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -11229,92 +11459,6 @@
       </c>
       <c r="J6">
         <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -11497,10 +11641,10 @@
         <v>28</v>
       </c>
       <c r="G7">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H7">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I7">
         <v>47</v>
@@ -11526,7 +11670,7 @@
         <v>307</v>
       </c>
       <c r="F8">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="G8">
         <v>110</v>
@@ -11558,13 +11702,13 @@
         <v>356</v>
       </c>
       <c r="F9">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="G9">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="H9">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I9">
         <v>174</v>
@@ -11579,6 +11723,92 @@
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I7"/>
   <sheetViews>
@@ -11735,227 +11965,6 @@
       </c>
       <c r="I7">
         <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>3</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>6</v>
-      </c>
-      <c r="C6">
-        <v>7</v>
-      </c>
-      <c r="D6">
-        <v>12</v>
-      </c>
-      <c r="E6">
-        <v>4</v>
-      </c>
-      <c r="F6">
-        <v>14</v>
-      </c>
-      <c r="G6">
-        <v>8</v>
-      </c>
-      <c r="H6">
-        <v>5</v>
-      </c>
-      <c r="I6">
-        <v>11</v>
-      </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>11</v>
-      </c>
-      <c r="C7">
-        <v>12</v>
-      </c>
-      <c r="D7">
-        <v>16</v>
-      </c>
-      <c r="E7">
-        <v>12</v>
-      </c>
-      <c r="F7">
-        <v>17</v>
-      </c>
-      <c r="G7">
-        <v>19</v>
-      </c>
-      <c r="H7">
-        <v>2</v>
-      </c>
-      <c r="I7">
-        <v>6</v>
-      </c>
-      <c r="J7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8">
-        <v>18</v>
-      </c>
-      <c r="C8">
-        <v>20</v>
-      </c>
-      <c r="D8">
-        <v>29</v>
-      </c>
-      <c r="E8">
-        <v>18</v>
-      </c>
-      <c r="F8">
-        <v>33</v>
-      </c>
-      <c r="G8">
-        <v>30</v>
-      </c>
-      <c r="H8">
-        <v>12</v>
-      </c>
-      <c r="I8">
-        <v>20</v>
-      </c>
-      <c r="J8">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -12071,7 +12080,7 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -12080,7 +12089,7 @@
         <v>3</v>
       </c>
       <c r="E5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F5">
         <v>5</v>
@@ -12089,7 +12098,7 @@
         <v>6</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I5">
         <v>3</v>
@@ -12135,7 +12144,7 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C7">
         <v>20</v>
@@ -12144,7 +12153,7 @@
         <v>12</v>
       </c>
       <c r="E7">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F7">
         <v>11</v>
@@ -12153,7 +12162,7 @@
         <v>25</v>
       </c>
       <c r="H7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I7">
         <v>11</v>
@@ -12807,7 +12816,7 @@
         <v>3</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -12865,7 +12874,7 @@
         <v>8</v>
       </c>
       <c r="H7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I7">
         <v>4</v>
@@ -13579,10 +13588,10 @@
         <v>5</v>
       </c>
       <c r="G6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I6">
         <v>12</v>
@@ -13605,7 +13614,7 @@
         <v>22</v>
       </c>
       <c r="E7">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F7">
         <v>21</v>
@@ -13637,16 +13646,16 @@
         <v>41</v>
       </c>
       <c r="E8">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F8">
         <v>42</v>
       </c>
       <c r="G8">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H8">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I8">
         <v>45</v>
@@ -13780,7 +13789,7 @@
         <v>6</v>
       </c>
       <c r="G5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H5">
         <v>5</v>
@@ -13815,7 +13824,7 @@
         <v>13</v>
       </c>
       <c r="I6">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J6">
         <v>5</v>
@@ -13841,13 +13850,13 @@
         <v>54</v>
       </c>
       <c r="G7">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H7">
         <v>7</v>
       </c>
       <c r="I7">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J7">
         <v>21</v>
@@ -15180,7 +15189,7 @@
         <v>2</v>
       </c>
       <c r="I5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J5">
         <v>2</v>
@@ -15212,7 +15221,7 @@
         <v>4</v>
       </c>
       <c r="I6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J6">
         <v>2</v>
@@ -15611,7 +15620,7 @@
         <v>2</v>
       </c>
       <c r="G6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I6">
         <v>3</v>
@@ -15640,7 +15649,7 @@
         <v>2</v>
       </c>
       <c r="G7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H7">
         <v>2</v>
@@ -15894,7 +15903,7 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -15917,7 +15926,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -16141,7 +16150,7 @@
         <v>7</v>
       </c>
       <c r="E6">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F6">
         <v>2</v>
@@ -16170,7 +16179,7 @@
         <v>8</v>
       </c>
       <c r="E7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F7">
         <v>3</v>
@@ -16328,7 +16337,7 @@
         <v>10</v>
       </c>
       <c r="E5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F5">
         <v>6</v>
@@ -16360,7 +16369,7 @@
         <v>15</v>
       </c>
       <c r="E6">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F6">
         <v>12</v>
@@ -16484,7 +16493,7 @@
         <v>2</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -16510,7 +16519,7 @@
         <v>2</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G7">
         <v>2</v>
@@ -16759,6 +16768,9 @@
       <c r="B3">
         <v>2</v>
       </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
       <c r="D3">
         <v>1</v>
       </c>
@@ -16771,7 +16783,7 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -17285,7 +17297,7 @@
         <v>18</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H5">
         <v>2</v>
@@ -17317,7 +17329,7 @@
         <v>23</v>
       </c>
       <c r="G6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H6">
         <v>2</v>
@@ -18517,13 +18529,13 @@
 
 <file path=xl/worksheets/sheet97.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" customWidth="1"/>
     <col min="3" max="3" width="4.7109375" customWidth="1"/>
     <col min="4" max="4" width="4.7109375" customWidth="1"/>
@@ -18545,34 +18557,42 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="D2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="D3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add data for 2023-07-03
</commit_message>
<xml_diff>
--- a/output/cta-index-crime-ytd.xlsx
+++ b/output/cta-index-crime-ytd.xlsx
@@ -29,8 +29,8 @@
     <sheet name="Jefferson Park" sheetId="20" r:id="rId20"/>
     <sheet name="Fuller Park" sheetId="21" r:id="rId21"/>
     <sheet name="Chinatown" sheetId="22" r:id="rId22"/>
-    <sheet name="Austin" sheetId="23" r:id="rId23"/>
-    <sheet name="Belmont Cragin" sheetId="24" r:id="rId24"/>
+    <sheet name="Belmont Cragin" sheetId="23" r:id="rId23"/>
+    <sheet name="Austin" sheetId="24" r:id="rId24"/>
     <sheet name="Old Town" sheetId="25" r:id="rId25"/>
     <sheet name="Hyde Park" sheetId="26" r:id="rId26"/>
     <sheet name="United Center" sheetId="27" r:id="rId27"/>
@@ -41,25 +41,25 @@
     <sheet name="New City" sheetId="32" r:id="rId32"/>
     <sheet name="Lake View" sheetId="33" r:id="rId33"/>
     <sheet name="Washington Heights" sheetId="34" r:id="rId34"/>
-    <sheet name="West Loop" sheetId="35" r:id="rId35"/>
+    <sheet name="North Lawndale" sheetId="35" r:id="rId35"/>
     <sheet name="Sheffield &amp; DePaul" sheetId="36" r:id="rId36"/>
     <sheet name="West Pullman" sheetId="37" r:id="rId37"/>
     <sheet name="North Center" sheetId="38" r:id="rId38"/>
     <sheet name="Norwood Park" sheetId="39" r:id="rId39"/>
     <sheet name="Wrigleyville" sheetId="40" r:id="rId40"/>
     <sheet name="Bucktown" sheetId="41" r:id="rId41"/>
-    <sheet name="Rogers Park" sheetId="42" r:id="rId42"/>
-    <sheet name="West Lawn" sheetId="43" r:id="rId43"/>
-    <sheet name="Wicker Park" sheetId="44" r:id="rId44"/>
-    <sheet name="Ukrainian Village" sheetId="45" r:id="rId45"/>
-    <sheet name="Little Italy, UIC" sheetId="46" r:id="rId46"/>
-    <sheet name="Archer Heights" sheetId="47" r:id="rId47"/>
-    <sheet name="Bridgeport" sheetId="48" r:id="rId48"/>
-    <sheet name="Montclare" sheetId="49" r:id="rId49"/>
-    <sheet name="O'Hare" sheetId="50" r:id="rId50"/>
-    <sheet name="Grant Park" sheetId="51" r:id="rId51"/>
-    <sheet name="Lincoln Park" sheetId="52" r:id="rId52"/>
-    <sheet name="North Lawndale" sheetId="53" r:id="rId53"/>
+    <sheet name="West Loop" sheetId="42" r:id="rId42"/>
+    <sheet name="Rogers Park" sheetId="43" r:id="rId43"/>
+    <sheet name="West Lawn" sheetId="44" r:id="rId44"/>
+    <sheet name="Wicker Park" sheetId="45" r:id="rId45"/>
+    <sheet name="Ukrainian Village" sheetId="46" r:id="rId46"/>
+    <sheet name="Little Italy, UIC" sheetId="47" r:id="rId47"/>
+    <sheet name="Archer Heights" sheetId="48" r:id="rId48"/>
+    <sheet name="Bridgeport" sheetId="49" r:id="rId49"/>
+    <sheet name="Montclare" sheetId="50" r:id="rId50"/>
+    <sheet name="O'Hare" sheetId="51" r:id="rId51"/>
+    <sheet name="Grant Park" sheetId="52" r:id="rId52"/>
+    <sheet name="Lincoln Park" sheetId="53" r:id="rId53"/>
     <sheet name="Auburn Gresham" sheetId="54" r:id="rId54"/>
     <sheet name="Brighton Park" sheetId="55" r:id="rId55"/>
     <sheet name="Logan Square" sheetId="56" r:id="rId56"/>
@@ -6523,6 +6523,145 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -6756,145 +6895,6 @@
       </c>
       <c r="J8">
         <v>40</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6">
-        <v>3</v>
-      </c>
-      <c r="F6">
-        <v>3</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <v>6</v>
-      </c>
-      <c r="D7">
-        <v>3</v>
-      </c>
-      <c r="E7">
-        <v>5</v>
-      </c>
-      <c r="F7">
-        <v>3</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -8971,7 +8971,7 @@
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -9025,7 +9025,13 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
         <v>1</v>
       </c>
       <c r="G2">
@@ -9042,134 +9048,141 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3">
-        <v>2</v>
+      <c r="C3">
+        <v>1</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
       <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
         <v>1</v>
       </c>
       <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="I4">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5">
+        <v>5</v>
+      </c>
+      <c r="H5">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6">
         <v>7</v>
       </c>
       <c r="D6">
+        <v>12</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>15</v>
+      </c>
+      <c r="G6">
+        <v>8</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="I6">
+        <v>11</v>
+      </c>
+      <c r="J6">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>13</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="E7">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="G7">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="H7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I7">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J7">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C8">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="D8">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="E8">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F8">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="G8">
+        <v>31</v>
+      </c>
+      <c r="H8">
         <v>12</v>
       </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
       <c r="I8">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>14</v>
-      </c>
-      <c r="C9">
-        <v>7</v>
-      </c>
-      <c r="D9">
-        <v>22</v>
-      </c>
-      <c r="E9">
-        <v>19</v>
-      </c>
-      <c r="F9">
-        <v>28</v>
-      </c>
-      <c r="G9">
-        <v>18</v>
-      </c>
-      <c r="H9">
-        <v>8</v>
-      </c>
-      <c r="I9">
-        <v>21</v>
-      </c>
-      <c r="J9">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -10337,6 +10350,214 @@
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>16</v>
+      </c>
+      <c r="E8">
+        <v>15</v>
+      </c>
+      <c r="F8">
+        <v>25</v>
+      </c>
+      <c r="G8">
+        <v>12</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>15</v>
+      </c>
+      <c r="J8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>14</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>22</v>
+      </c>
+      <c r="E9">
+        <v>19</v>
+      </c>
+      <c r="F9">
+        <v>28</v>
+      </c>
+      <c r="G9">
+        <v>18</v>
+      </c>
+      <c r="H9">
+        <v>8</v>
+      </c>
+      <c r="I9">
+        <v>21</v>
+      </c>
+      <c r="J9">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -10547,7 +10768,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G5"/>
   <sheetViews>
@@ -10651,7 +10872,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -10814,7 +11035,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -10913,7 +11134,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J7"/>
   <sheetViews>
@@ -11111,7 +11332,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F6"/>
   <sheetViews>
@@ -11210,7 +11431,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J5"/>
   <sheetViews>
@@ -11358,82 +11579,6 @@
       </c>
       <c r="J5">
         <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -11699,6 +11844,82 @@
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -11857,7 +12078,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -11943,7 +12164,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I7"/>
   <sheetViews>
@@ -12100,227 +12321,6 @@
       </c>
       <c r="I7">
         <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>3</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>6</v>
-      </c>
-      <c r="C6">
-        <v>7</v>
-      </c>
-      <c r="D6">
-        <v>12</v>
-      </c>
-      <c r="E6">
-        <v>4</v>
-      </c>
-      <c r="F6">
-        <v>15</v>
-      </c>
-      <c r="G6">
-        <v>8</v>
-      </c>
-      <c r="H6">
-        <v>5</v>
-      </c>
-      <c r="I6">
-        <v>11</v>
-      </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>11</v>
-      </c>
-      <c r="C7">
-        <v>13</v>
-      </c>
-      <c r="D7">
-        <v>16</v>
-      </c>
-      <c r="E7">
-        <v>12</v>
-      </c>
-      <c r="F7">
-        <v>17</v>
-      </c>
-      <c r="G7">
-        <v>20</v>
-      </c>
-      <c r="H7">
-        <v>2</v>
-      </c>
-      <c r="I7">
-        <v>6</v>
-      </c>
-      <c r="J7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8">
-        <v>18</v>
-      </c>
-      <c r="C8">
-        <v>21</v>
-      </c>
-      <c r="D8">
-        <v>29</v>
-      </c>
-      <c r="E8">
-        <v>18</v>
-      </c>
-      <c r="F8">
-        <v>35</v>
-      </c>
-      <c r="G8">
-        <v>31</v>
-      </c>
-      <c r="H8">
-        <v>12</v>
-      </c>
-      <c r="I8">
-        <v>20</v>
-      </c>
-      <c r="J8">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2023-07-05
</commit_message>
<xml_diff>
--- a/output/cta-index-crime-ytd.xlsx
+++ b/output/cta-index-crime-ytd.xlsx
@@ -29,38 +29,38 @@
     <sheet name="Jefferson Park" sheetId="20" r:id="rId20"/>
     <sheet name="Fuller Park" sheetId="21" r:id="rId21"/>
     <sheet name="Chinatown" sheetId="22" r:id="rId22"/>
-    <sheet name="Belmont Cragin" sheetId="23" r:id="rId23"/>
-    <sheet name="Austin" sheetId="24" r:id="rId24"/>
+    <sheet name="Austin" sheetId="23" r:id="rId23"/>
+    <sheet name="Belmont Cragin" sheetId="24" r:id="rId24"/>
     <sheet name="Old Town" sheetId="25" r:id="rId25"/>
     <sheet name="Hyde Park" sheetId="26" r:id="rId26"/>
     <sheet name="United Center" sheetId="27" r:id="rId27"/>
     <sheet name="Roseland" sheetId="28" r:id="rId28"/>
     <sheet name="Chatham" sheetId="29" r:id="rId29"/>
     <sheet name="Albany Park" sheetId="30" r:id="rId30"/>
-    <sheet name="Ashburn" sheetId="31" r:id="rId31"/>
-    <sheet name="New City" sheetId="32" r:id="rId32"/>
-    <sheet name="Rogers Park" sheetId="33" r:id="rId33"/>
+    <sheet name="Rogers Park" sheetId="31" r:id="rId31"/>
+    <sheet name="Ashburn" sheetId="32" r:id="rId32"/>
+    <sheet name="New City" sheetId="33" r:id="rId33"/>
     <sheet name="Lake View" sheetId="34" r:id="rId34"/>
     <sheet name="River North" sheetId="35" r:id="rId35"/>
     <sheet name="Washington Heights" sheetId="36" r:id="rId36"/>
-    <sheet name="North Lawndale" sheetId="37" r:id="rId37"/>
+    <sheet name="West Loop" sheetId="37" r:id="rId37"/>
     <sheet name="Sheffield &amp; DePaul" sheetId="38" r:id="rId38"/>
     <sheet name="West Pullman" sheetId="39" r:id="rId39"/>
     <sheet name="North Center" sheetId="40" r:id="rId40"/>
     <sheet name="Norwood Park" sheetId="41" r:id="rId41"/>
     <sheet name="Wrigleyville" sheetId="42" r:id="rId42"/>
     <sheet name="Bucktown" sheetId="43" r:id="rId43"/>
-    <sheet name="West Loop" sheetId="44" r:id="rId44"/>
-    <sheet name="West Lawn" sheetId="45" r:id="rId45"/>
-    <sheet name="Wicker Park" sheetId="46" r:id="rId46"/>
-    <sheet name="Ukrainian Village" sheetId="47" r:id="rId47"/>
-    <sheet name="Little Italy, UIC" sheetId="48" r:id="rId48"/>
-    <sheet name="Archer Heights" sheetId="49" r:id="rId49"/>
-    <sheet name="Bridgeport" sheetId="50" r:id="rId50"/>
-    <sheet name="Montclare" sheetId="51" r:id="rId51"/>
-    <sheet name="O'Hare" sheetId="52" r:id="rId52"/>
-    <sheet name="Grant Park" sheetId="53" r:id="rId53"/>
-    <sheet name="Lincoln Park" sheetId="54" r:id="rId54"/>
+    <sheet name="West Lawn" sheetId="44" r:id="rId44"/>
+    <sheet name="Wicker Park" sheetId="45" r:id="rId45"/>
+    <sheet name="Ukrainian Village" sheetId="46" r:id="rId46"/>
+    <sheet name="Little Italy, UIC" sheetId="47" r:id="rId47"/>
+    <sheet name="Archer Heights" sheetId="48" r:id="rId48"/>
+    <sheet name="Bridgeport" sheetId="49" r:id="rId49"/>
+    <sheet name="Montclare" sheetId="50" r:id="rId50"/>
+    <sheet name="O'Hare" sheetId="51" r:id="rId51"/>
+    <sheet name="Grant Park" sheetId="52" r:id="rId52"/>
+    <sheet name="Lincoln Park" sheetId="53" r:id="rId53"/>
+    <sheet name="North Lawndale" sheetId="54" r:id="rId54"/>
     <sheet name="Auburn Gresham" sheetId="55" r:id="rId55"/>
     <sheet name="Brighton Park" sheetId="56" r:id="rId56"/>
     <sheet name="Logan Square" sheetId="57" r:id="rId57"/>
@@ -6526,145 +6526,6 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6">
-        <v>3</v>
-      </c>
-      <c r="F6">
-        <v>3</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <v>6</v>
-      </c>
-      <c r="D7">
-        <v>3</v>
-      </c>
-      <c r="E7">
-        <v>5</v>
-      </c>
-      <c r="F7">
-        <v>3</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -6898,6 +6759,145 @@
       </c>
       <c r="J8">
         <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -8262,13 +8262,13 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" customWidth="1"/>
     <col min="3" max="3" width="4.7109375" customWidth="1"/>
     <col min="4" max="4" width="4.7109375" customWidth="1"/>
@@ -8317,12 +8317,15 @@
         <v>1</v>
       </c>
       <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="F2">
         <v>1</v>
       </c>
       <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="I2">
         <v>1</v>
       </c>
     </row>
@@ -8330,10 +8333,25 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
       <c r="D3">
         <v>1</v>
       </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
       <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
@@ -8342,74 +8360,114 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="H4">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5">
-        <v>4</v>
-      </c>
-      <c r="G5">
-        <v>3</v>
-      </c>
-      <c r="H5">
-        <v>2</v>
-      </c>
-      <c r="J5">
+        <v>7</v>
+      </c>
+      <c r="I5">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>8</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>9</v>
+      </c>
+      <c r="I6">
+        <v>6</v>
+      </c>
+      <c r="J6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>18</v>
+      </c>
+      <c r="C7">
+        <v>31</v>
+      </c>
+      <c r="D7">
+        <v>23</v>
+      </c>
+      <c r="E7">
+        <v>35</v>
+      </c>
+      <c r="F7">
+        <v>14</v>
+      </c>
+      <c r="G7">
+        <v>16</v>
+      </c>
+      <c r="H7">
+        <v>17</v>
+      </c>
+      <c r="I7">
+        <v>13</v>
+      </c>
+      <c r="J7">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>3</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6">
-        <v>5</v>
-      </c>
-      <c r="G6">
-        <v>5</v>
-      </c>
-      <c r="H6">
-        <v>2</v>
-      </c>
-      <c r="I6">
-        <v>2</v>
-      </c>
-      <c r="J6">
-        <v>2</v>
+      <c r="B8">
+        <v>19</v>
+      </c>
+      <c r="C8">
+        <v>38</v>
+      </c>
+      <c r="D8">
+        <v>30</v>
+      </c>
+      <c r="E8">
+        <v>43</v>
+      </c>
+      <c r="F8">
+        <v>24</v>
+      </c>
+      <c r="G8">
+        <v>24</v>
+      </c>
+      <c r="H8">
+        <v>28</v>
+      </c>
+      <c r="I8">
+        <v>21</v>
+      </c>
+      <c r="J8">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -8473,13 +8531,13 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="H2">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="I2">
         <v>1</v>
       </c>
     </row>
@@ -8487,31 +8545,25 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
+      <c r="D3">
+        <v>1</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
       <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -8524,20 +8576,20 @@
       <c r="B5">
         <v>2</v>
       </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
       <c r="D5">
         <v>2</v>
       </c>
       <c r="E5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G5">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -8548,31 +8600,31 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C6">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E6">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F6">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G6">
         <v>5</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J6">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -8582,13 +8634,13 @@
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" customWidth="1"/>
     <col min="3" max="3" width="4.7109375" customWidth="1"/>
     <col min="4" max="4" width="4.7109375" customWidth="1"/>
@@ -8636,16 +8688,13 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>2</v>
+      <c r="B2">
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
         <v>1</v>
       </c>
     </row>
@@ -8653,141 +8702,92 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
+      <c r="B3">
         <v>1</v>
       </c>
       <c r="E3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="G3">
-        <v>4</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
       <c r="J3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="I4">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="J5">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F6">
         <v>8</v>
       </c>
       <c r="G6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H6">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I6">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="J6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>18</v>
-      </c>
-      <c r="C7">
-        <v>31</v>
-      </c>
-      <c r="D7">
-        <v>23</v>
-      </c>
-      <c r="E7">
-        <v>35</v>
-      </c>
-      <c r="F7">
-        <v>14</v>
-      </c>
-      <c r="G7">
-        <v>16</v>
-      </c>
-      <c r="H7">
-        <v>17</v>
-      </c>
-      <c r="I7">
-        <v>13</v>
-      </c>
-      <c r="J7">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8">
-        <v>19</v>
-      </c>
-      <c r="C8">
-        <v>38</v>
-      </c>
-      <c r="D8">
-        <v>30</v>
-      </c>
-      <c r="E8">
-        <v>43</v>
-      </c>
-      <c r="F8">
-        <v>24</v>
-      </c>
-      <c r="G8">
-        <v>24</v>
-      </c>
-      <c r="H8">
-        <v>28</v>
-      </c>
-      <c r="I8">
-        <v>21</v>
-      </c>
-      <c r="J8">
-        <v>27</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -9387,7 +9387,7 @@
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -9441,13 +9441,7 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
+      <c r="B2">
         <v>1</v>
       </c>
       <c r="G2">
@@ -9464,141 +9458,137 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>1</v>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
       <c r="G3">
-        <v>2</v>
-      </c>
-      <c r="H3">
         <v>1</v>
       </c>
       <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="F4">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5">
+        <v>6</v>
+      </c>
+      <c r="I5">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
         <v>7</v>
       </c>
-      <c r="C6">
-        <v>7</v>
-      </c>
       <c r="D6">
-        <v>12</v>
-      </c>
-      <c r="E6">
-        <v>4</v>
-      </c>
-      <c r="F6">
-        <v>15</v>
-      </c>
-      <c r="G6">
-        <v>8</v>
-      </c>
-      <c r="H6">
-        <v>5</v>
-      </c>
-      <c r="I6">
-        <v>11</v>
-      </c>
-      <c r="J6">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7">
-        <v>11</v>
-      </c>
-      <c r="C7">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D7">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="E7">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="F7">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="G7">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="H7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I7">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="J7">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>16</v>
+      </c>
+      <c r="E8">
+        <v>15</v>
+      </c>
+      <c r="F8">
+        <v>25</v>
+      </c>
+      <c r="G8">
+        <v>12</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>15</v>
+      </c>
+      <c r="J8">
         <v>10</v>
       </c>
-      <c r="B8">
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>22</v>
+      </c>
+      <c r="E9">
         <v>19</v>
       </c>
-      <c r="C8">
+      <c r="F9">
+        <v>28</v>
+      </c>
+      <c r="G9">
+        <v>18</v>
+      </c>
+      <c r="H9">
+        <v>8</v>
+      </c>
+      <c r="I9">
         <v>21</v>
       </c>
-      <c r="D8">
-        <v>29</v>
-      </c>
-      <c r="E8">
-        <v>18</v>
-      </c>
-      <c r="F8">
-        <v>35</v>
-      </c>
-      <c r="G8">
-        <v>31</v>
-      </c>
-      <c r="H8">
+      <c r="J9">
         <v>12</v>
-      </c>
-      <c r="I8">
-        <v>20</v>
-      </c>
-      <c r="J8">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -10777,217 +10767,6 @@
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>3</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>4</v>
-      </c>
-      <c r="D7">
-        <v>3</v>
-      </c>
-      <c r="E7">
-        <v>3</v>
-      </c>
-      <c r="F7">
-        <v>2</v>
-      </c>
-      <c r="G7">
-        <v>4</v>
-      </c>
-      <c r="H7">
-        <v>4</v>
-      </c>
-      <c r="I7">
-        <v>3</v>
-      </c>
-      <c r="J7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <v>9</v>
-      </c>
-      <c r="C8">
-        <v>7</v>
-      </c>
-      <c r="D8">
-        <v>16</v>
-      </c>
-      <c r="E8">
-        <v>15</v>
-      </c>
-      <c r="F8">
-        <v>25</v>
-      </c>
-      <c r="G8">
-        <v>12</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8">
-        <v>15</v>
-      </c>
-      <c r="J8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>15</v>
-      </c>
-      <c r="C9">
-        <v>7</v>
-      </c>
-      <c r="D9">
-        <v>22</v>
-      </c>
-      <c r="E9">
-        <v>19</v>
-      </c>
-      <c r="F9">
-        <v>28</v>
-      </c>
-      <c r="G9">
-        <v>18</v>
-      </c>
-      <c r="H9">
-        <v>8</v>
-      </c>
-      <c r="I9">
-        <v>21</v>
-      </c>
-      <c r="J9">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -11090,7 +10869,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -11253,7 +11032,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -11352,7 +11131,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J7"/>
   <sheetViews>
@@ -11550,7 +11329,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F6"/>
   <sheetViews>
@@ -11642,6 +11421,161 @@
       </c>
       <c r="F6">
         <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>6</v>
+      </c>
+      <c r="G5">
+        <v>6</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -11907,161 +11841,6 @@
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>6</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4">
-        <v>6</v>
-      </c>
-      <c r="G4">
-        <v>4</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>9</v>
-      </c>
-      <c r="E5">
-        <v>4</v>
-      </c>
-      <c r="F5">
-        <v>6</v>
-      </c>
-      <c r="G5">
-        <v>6</v>
-      </c>
-      <c r="H5">
-        <v>2</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -12136,7 +11915,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -12296,7 +12075,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -12382,7 +12161,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I7"/>
   <sheetViews>
@@ -12539,6 +12318,227 @@
       </c>
       <c r="I7">
         <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>12</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>15</v>
+      </c>
+      <c r="G6">
+        <v>8</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="I6">
+        <v>11</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>13</v>
+      </c>
+      <c r="D7">
+        <v>16</v>
+      </c>
+      <c r="E7">
+        <v>12</v>
+      </c>
+      <c r="F7">
+        <v>17</v>
+      </c>
+      <c r="G7">
+        <v>20</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>6</v>
+      </c>
+      <c r="J7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>19</v>
+      </c>
+      <c r="C8">
+        <v>21</v>
+      </c>
+      <c r="D8">
+        <v>29</v>
+      </c>
+      <c r="E8">
+        <v>18</v>
+      </c>
+      <c r="F8">
+        <v>35</v>
+      </c>
+      <c r="G8">
+        <v>31</v>
+      </c>
+      <c r="H8">
+        <v>12</v>
+      </c>
+      <c r="I8">
+        <v>20</v>
+      </c>
+      <c r="J8">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2023-07-20
</commit_message>
<xml_diff>
--- a/output/cta-index-crime-ytd.xlsx
+++ b/output/cta-index-crime-ytd.xlsx
@@ -47,8 +47,8 @@
     <sheet name="West Elsdon" sheetId="38" r:id="rId38"/>
     <sheet name="Near South Side" sheetId="39" r:id="rId39"/>
     <sheet name="Logan Square" sheetId="40" r:id="rId40"/>
-    <sheet name="Little Italy, UIC" sheetId="41" r:id="rId41"/>
-    <sheet name="Bridgeport" sheetId="42" r:id="rId42"/>
+    <sheet name="Bridgeport" sheetId="41" r:id="rId41"/>
+    <sheet name="Little Italy, UIC" sheetId="42" r:id="rId42"/>
     <sheet name="Irving Park" sheetId="43" r:id="rId43"/>
     <sheet name="Wicker Park" sheetId="44" r:id="rId44"/>
     <sheet name="Lincoln Park" sheetId="45" r:id="rId45"/>
@@ -10175,6 +10175,161 @@
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>7</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>7</v>
+      </c>
+      <c r="G5">
+        <v>6</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -10370,161 +10525,6 @@
       </c>
       <c r="J7">
         <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>6</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4">
-        <v>7</v>
-      </c>
-      <c r="G4">
-        <v>4</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>9</v>
-      </c>
-      <c r="E5">
-        <v>4</v>
-      </c>
-      <c r="F5">
-        <v>7</v>
-      </c>
-      <c r="G5">
-        <v>6</v>
-      </c>
-      <c r="H5">
-        <v>2</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2023-08-03
</commit_message>
<xml_diff>
--- a/output/cta-index-crime-ytd.xlsx
+++ b/output/cta-index-crime-ytd.xlsx
@@ -30,26 +30,26 @@
     <sheet name="Ashburn" sheetId="21" r:id="rId21"/>
     <sheet name="New City" sheetId="22" r:id="rId22"/>
     <sheet name="Lower West Side" sheetId="23" r:id="rId23"/>
-    <sheet name="Irving Park" sheetId="24" r:id="rId24"/>
-    <sheet name="Rogers Park" sheetId="25" r:id="rId25"/>
-    <sheet name="Kenwood" sheetId="26" r:id="rId26"/>
-    <sheet name="Roseland" sheetId="27" r:id="rId27"/>
-    <sheet name="Austin" sheetId="28" r:id="rId28"/>
-    <sheet name="Hyde Park" sheetId="29" r:id="rId29"/>
-    <sheet name="River North" sheetId="30" r:id="rId30"/>
-    <sheet name="Fuller Park" sheetId="31" r:id="rId31"/>
-    <sheet name="Old Town" sheetId="32" r:id="rId32"/>
-    <sheet name="Printers Row" sheetId="33" r:id="rId33"/>
-    <sheet name="Lincoln Park" sheetId="34" r:id="rId34"/>
-    <sheet name="Chicago Lawn" sheetId="35" r:id="rId35"/>
-    <sheet name="Uptown" sheetId="36" r:id="rId36"/>
-    <sheet name="Wrigleyville" sheetId="37" r:id="rId37"/>
-    <sheet name="Logan Square" sheetId="38" r:id="rId38"/>
-    <sheet name="Edgewater" sheetId="39" r:id="rId39"/>
-    <sheet name="South Chicago" sheetId="40" r:id="rId40"/>
-    <sheet name="West Elsdon" sheetId="41" r:id="rId41"/>
-    <sheet name="Little Italy, UIC" sheetId="42" r:id="rId42"/>
-    <sheet name="Sheffield &amp; DePaul" sheetId="43" r:id="rId43"/>
+    <sheet name="South Chicago" sheetId="24" r:id="rId24"/>
+    <sheet name="Lincoln Park" sheetId="25" r:id="rId25"/>
+    <sheet name="Sheffield &amp; DePaul" sheetId="26" r:id="rId26"/>
+    <sheet name="Rogers Park" sheetId="27" r:id="rId27"/>
+    <sheet name="Edgewater" sheetId="28" r:id="rId28"/>
+    <sheet name="Kenwood" sheetId="29" r:id="rId29"/>
+    <sheet name="Roseland" sheetId="30" r:id="rId30"/>
+    <sheet name="Austin" sheetId="31" r:id="rId31"/>
+    <sheet name="Hyde Park" sheetId="32" r:id="rId32"/>
+    <sheet name="River North" sheetId="33" r:id="rId33"/>
+    <sheet name="Fuller Park" sheetId="34" r:id="rId34"/>
+    <sheet name="Old Town" sheetId="35" r:id="rId35"/>
+    <sheet name="Printers Row" sheetId="36" r:id="rId36"/>
+    <sheet name="Chicago Lawn" sheetId="37" r:id="rId37"/>
+    <sheet name="Uptown" sheetId="38" r:id="rId38"/>
+    <sheet name="Wrigleyville" sheetId="39" r:id="rId39"/>
+    <sheet name="Logan Square" sheetId="40" r:id="rId40"/>
+    <sheet name="Irving Park" sheetId="41" r:id="rId41"/>
+    <sheet name="West Elsdon" sheetId="42" r:id="rId42"/>
+    <sheet name="Little Italy, UIC" sheetId="43" r:id="rId43"/>
     <sheet name="Bucktown" sheetId="44" r:id="rId44"/>
     <sheet name="Woodlawn" sheetId="45" r:id="rId45"/>
     <sheet name="Bridgeport" sheetId="46" r:id="rId46"/>
@@ -6752,6 +6752,193 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
+      <c r="F5">
+        <v>6</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>13</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6">
+        <v>8</v>
+      </c>
+      <c r="I6">
+        <v>6</v>
+      </c>
+      <c r="J6">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -6806,13 +6993,7 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="I2">
+      <c r="D2">
         <v>1</v>
       </c>
       <c r="J2">
@@ -6823,27 +7004,21 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
+      <c r="F3">
         <v>1</v>
       </c>
       <c r="G3">
-        <v>2</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4">
+      <c r="B4">
         <v>1</v>
       </c>
     </row>
@@ -6851,29 +7026,26 @@
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
       <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
         <v>2</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I5">
         <v>1</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -6881,31 +7053,28 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D6">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E6">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F6">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G6">
-        <v>8</v>
-      </c>
-      <c r="H6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I6">
         <v>4</v>
       </c>
       <c r="J6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -6913,252 +7082,31 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C7">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D7">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E7">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F7">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="G7">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I7">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J7">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>7</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>4</v>
-      </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>7</v>
-      </c>
-      <c r="D6">
-        <v>7</v>
-      </c>
-      <c r="E6">
-        <v>3</v>
-      </c>
-      <c r="F6">
-        <v>10</v>
-      </c>
-      <c r="G6">
-        <v>4</v>
-      </c>
-      <c r="H6">
-        <v>9</v>
-      </c>
-      <c r="I6">
-        <v>10</v>
-      </c>
-      <c r="J6">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>26</v>
-      </c>
-      <c r="C7">
-        <v>37</v>
-      </c>
-      <c r="D7">
-        <v>26</v>
-      </c>
-      <c r="E7">
-        <v>43</v>
-      </c>
-      <c r="F7">
-        <v>19</v>
-      </c>
-      <c r="G7">
-        <v>19</v>
-      </c>
-      <c r="H7">
-        <v>17</v>
-      </c>
-      <c r="I7">
-        <v>16</v>
-      </c>
-      <c r="J7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8">
-        <v>28</v>
-      </c>
-      <c r="C8">
-        <v>47</v>
-      </c>
-      <c r="D8">
-        <v>35</v>
-      </c>
-      <c r="E8">
-        <v>54</v>
-      </c>
-      <c r="F8">
-        <v>31</v>
-      </c>
-      <c r="G8">
-        <v>28</v>
-      </c>
-      <c r="H8">
-        <v>29</v>
-      </c>
-      <c r="I8">
-        <v>29</v>
-      </c>
-      <c r="J8">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -7222,15 +7170,42 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
       <c r="H2">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G3">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
         <v>1</v>
       </c>
     </row>
@@ -7238,15 +7213,42 @@
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
       <c r="I4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
       <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>6</v>
+      </c>
+      <c r="J5">
         <v>1</v>
       </c>
     </row>
@@ -7255,25 +7257,31 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E6">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="F6">
-        <v>3</v>
+        <v>21</v>
+      </c>
+      <c r="G6">
+        <v>11</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
       </c>
       <c r="J6">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -7281,31 +7289,31 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E7">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="F7">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="G7">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="H7">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="J7">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -7314,252 +7322,6 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
-      <c r="H2">
-        <v>2</v>
-      </c>
-      <c r="I2">
-        <v>5</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>4</v>
-      </c>
-      <c r="F3">
-        <v>4</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>4</v>
-      </c>
-      <c r="I3">
-        <v>6</v>
-      </c>
-      <c r="J3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>12</v>
-      </c>
-      <c r="C8">
-        <v>11</v>
-      </c>
-      <c r="D8">
-        <v>3</v>
-      </c>
-      <c r="E8">
-        <v>10</v>
-      </c>
-      <c r="F8">
-        <v>4</v>
-      </c>
-      <c r="G8">
-        <v>9</v>
-      </c>
-      <c r="H8">
-        <v>10</v>
-      </c>
-      <c r="I8">
-        <v>16</v>
-      </c>
-      <c r="J8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>28</v>
-      </c>
-      <c r="C9">
-        <v>28</v>
-      </c>
-      <c r="D9">
-        <v>24</v>
-      </c>
-      <c r="E9">
-        <v>28</v>
-      </c>
-      <c r="F9">
-        <v>27</v>
-      </c>
-      <c r="G9">
-        <v>18</v>
-      </c>
-      <c r="H9">
-        <v>18</v>
-      </c>
-      <c r="I9">
-        <v>23</v>
-      </c>
-      <c r="J9">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10">
-        <v>42</v>
-      </c>
-      <c r="C10">
-        <v>44</v>
-      </c>
-      <c r="D10">
-        <v>31</v>
-      </c>
-      <c r="E10">
-        <v>45</v>
-      </c>
-      <c r="F10">
-        <v>37</v>
-      </c>
-      <c r="G10">
-        <v>30</v>
-      </c>
-      <c r="H10">
-        <v>34</v>
-      </c>
-      <c r="I10">
-        <v>51</v>
-      </c>
-      <c r="J10">
-        <v>43</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J8"/>
   <sheetViews>
@@ -7615,89 +7377,68 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>4</v>
-      </c>
       <c r="C2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="H2">
-        <v>2</v>
-      </c>
       <c r="I2">
-        <v>3</v>
-      </c>
-      <c r="J2">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
       <c r="C3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <v>4</v>
       </c>
       <c r="H3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J3">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="H4">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>2</v>
+        <v>7</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -7705,31 +7446,31 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C6">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D6">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E6">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="F6">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G6">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="H6">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="I6">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J6">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -7737,31 +7478,31 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D7">
+        <v>26</v>
+      </c>
+      <c r="E7">
+        <v>43</v>
+      </c>
+      <c r="F7">
+        <v>19</v>
+      </c>
+      <c r="G7">
+        <v>19</v>
+      </c>
+      <c r="H7">
         <v>17</v>
       </c>
-      <c r="E7">
-        <v>34</v>
-      </c>
-      <c r="F7">
-        <v>51</v>
-      </c>
-      <c r="G7">
-        <v>49</v>
-      </c>
-      <c r="H7">
-        <v>18</v>
-      </c>
       <c r="I7">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="J7">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -7769,31 +7510,31 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="C8">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="D8">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E8">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="F8">
-        <v>84</v>
+        <v>31</v>
       </c>
       <c r="G8">
-        <v>70</v>
+        <v>28</v>
       </c>
       <c r="H8">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="I8">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="J8">
-        <v>44</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -7801,7 +7542,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -7857,7 +7598,22 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
       <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2">
         <v>1</v>
       </c>
     </row>
@@ -7865,17 +7621,17 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -7883,25 +7639,31 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J4">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -7909,31 +7671,31 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E5">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F5">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J5">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -7941,31 +7703,178 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="E6">
+        <v>16</v>
+      </c>
+      <c r="F6">
+        <v>17</v>
+      </c>
+      <c r="G6">
+        <v>13</v>
+      </c>
+      <c r="H6">
+        <v>12</v>
+      </c>
+      <c r="I6">
+        <v>14</v>
+      </c>
+      <c r="J6">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
       <c r="F6">
-        <v>4</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H6">
-        <v>5</v>
-      </c>
-      <c r="I6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -8168,6 +8077,666 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <v>6</v>
+      </c>
+      <c r="J3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>11</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>10</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+      <c r="G8">
+        <v>9</v>
+      </c>
+      <c r="H8">
+        <v>10</v>
+      </c>
+      <c r="I8">
+        <v>16</v>
+      </c>
+      <c r="J8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>28</v>
+      </c>
+      <c r="C9">
+        <v>28</v>
+      </c>
+      <c r="D9">
+        <v>24</v>
+      </c>
+      <c r="E9">
+        <v>28</v>
+      </c>
+      <c r="F9">
+        <v>27</v>
+      </c>
+      <c r="G9">
+        <v>18</v>
+      </c>
+      <c r="H9">
+        <v>18</v>
+      </c>
+      <c r="I9">
+        <v>23</v>
+      </c>
+      <c r="J9">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>42</v>
+      </c>
+      <c r="C10">
+        <v>44</v>
+      </c>
+      <c r="D10">
+        <v>31</v>
+      </c>
+      <c r="E10">
+        <v>45</v>
+      </c>
+      <c r="F10">
+        <v>37</v>
+      </c>
+      <c r="G10">
+        <v>30</v>
+      </c>
+      <c r="H10">
+        <v>34</v>
+      </c>
+      <c r="I10">
+        <v>51</v>
+      </c>
+      <c r="J10">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>6</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+      <c r="J2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>22</v>
+      </c>
+      <c r="D6">
+        <v>14</v>
+      </c>
+      <c r="E6">
+        <v>18</v>
+      </c>
+      <c r="F6">
+        <v>22</v>
+      </c>
+      <c r="G6">
+        <v>16</v>
+      </c>
+      <c r="H6">
+        <v>19</v>
+      </c>
+      <c r="I6">
+        <v>13</v>
+      </c>
+      <c r="J6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>27</v>
+      </c>
+      <c r="C7">
+        <v>32</v>
+      </c>
+      <c r="D7">
+        <v>17</v>
+      </c>
+      <c r="E7">
+        <v>34</v>
+      </c>
+      <c r="F7">
+        <v>51</v>
+      </c>
+      <c r="G7">
+        <v>49</v>
+      </c>
+      <c r="H7">
+        <v>18</v>
+      </c>
+      <c r="I7">
+        <v>24</v>
+      </c>
+      <c r="J7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>49</v>
+      </c>
+      <c r="C8">
+        <v>62</v>
+      </c>
+      <c r="D8">
+        <v>39</v>
+      </c>
+      <c r="E8">
+        <v>60</v>
+      </c>
+      <c r="F8">
+        <v>84</v>
+      </c>
+      <c r="G8">
+        <v>70</v>
+      </c>
+      <c r="H8">
+        <v>42</v>
+      </c>
+      <c r="I8">
+        <v>44</v>
+      </c>
+      <c r="J8">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>9</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="J6">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -8370,7 +8939,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J9"/>
   <sheetViews>
@@ -8587,7 +9156,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J7"/>
   <sheetViews>
@@ -8791,7 +9360,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -8953,601 +9522,6 @@
       </c>
       <c r="J6">
         <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>4</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <v>7</v>
-      </c>
-      <c r="D6">
-        <v>10</v>
-      </c>
-      <c r="E6">
-        <v>3</v>
-      </c>
-      <c r="F6">
-        <v>10</v>
-      </c>
-      <c r="G6">
-        <v>4</v>
-      </c>
-      <c r="I6">
-        <v>4</v>
-      </c>
-      <c r="J6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>10</v>
-      </c>
-      <c r="C7">
-        <v>8</v>
-      </c>
-      <c r="D7">
-        <v>11</v>
-      </c>
-      <c r="E7">
-        <v>7</v>
-      </c>
-      <c r="F7">
-        <v>13</v>
-      </c>
-      <c r="G7">
-        <v>5</v>
-      </c>
-      <c r="H7">
-        <v>3</v>
-      </c>
-      <c r="I7">
-        <v>5</v>
-      </c>
-      <c r="J7">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>3</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>2</v>
-      </c>
-      <c r="J3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>7</v>
-      </c>
-      <c r="D5">
-        <v>6</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>3</v>
-      </c>
-      <c r="G5">
-        <v>3</v>
-      </c>
-      <c r="H5">
-        <v>3</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <v>11</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6">
-        <v>3</v>
-      </c>
-      <c r="F6">
-        <v>5</v>
-      </c>
-      <c r="G6">
-        <v>4</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6">
-        <v>3</v>
-      </c>
-      <c r="J6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>17</v>
-      </c>
-      <c r="C7">
-        <v>12</v>
-      </c>
-      <c r="D7">
-        <v>12</v>
-      </c>
-      <c r="E7">
-        <v>5</v>
-      </c>
-      <c r="F7">
-        <v>9</v>
-      </c>
-      <c r="G7">
-        <v>10</v>
-      </c>
-      <c r="H7">
-        <v>5</v>
-      </c>
-      <c r="I7">
-        <v>5</v>
-      </c>
-      <c r="J7">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
-      <c r="H2">
-        <v>5</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
-      <c r="G3">
-        <v>4</v>
-      </c>
-      <c r="I3">
-        <v>2</v>
-      </c>
-      <c r="J3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>5</v>
-      </c>
-      <c r="C7">
-        <v>5</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>4</v>
-      </c>
-      <c r="G7">
-        <v>10</v>
-      </c>
-      <c r="H7">
-        <v>6</v>
-      </c>
-      <c r="I7">
-        <v>4</v>
-      </c>
-      <c r="J7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <v>12</v>
-      </c>
-      <c r="C8">
-        <v>16</v>
-      </c>
-      <c r="D8">
-        <v>11</v>
-      </c>
-      <c r="E8">
-        <v>14</v>
-      </c>
-      <c r="F8">
-        <v>12</v>
-      </c>
-      <c r="G8">
-        <v>13</v>
-      </c>
-      <c r="H8">
-        <v>7</v>
-      </c>
-      <c r="I8">
-        <v>8</v>
-      </c>
-      <c r="J8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>18</v>
-      </c>
-      <c r="C9">
-        <v>24</v>
-      </c>
-      <c r="D9">
-        <v>13</v>
-      </c>
-      <c r="E9">
-        <v>20</v>
-      </c>
-      <c r="F9">
-        <v>19</v>
-      </c>
-      <c r="G9">
-        <v>29</v>
-      </c>
-      <c r="H9">
-        <v>18</v>
-      </c>
-      <c r="I9">
-        <v>15</v>
-      </c>
-      <c r="J9">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -9611,19 +9585,13 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
+      <c r="D2">
         <v>1</v>
       </c>
       <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="J2">
+        <v>3</v>
+      </c>
+      <c r="H2">
         <v>1</v>
       </c>
     </row>
@@ -9631,20 +9599,26 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
         <v>1</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -9659,20 +9633,23 @@
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5">
-        <v>2</v>
+      <c r="B5">
+        <v>7</v>
       </c>
       <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5">
         <v>1</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G5">
-        <v>2</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -9683,31 +9660,31 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C6">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D6">
         <v>4</v>
       </c>
       <c r="E6">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F6">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -9715,31 +9692,31 @@
         <v>10</v>
       </c>
       <c r="B7">
+        <v>17</v>
+      </c>
+      <c r="C7">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>12</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
         <v>9</v>
       </c>
-      <c r="C7">
-        <v>9</v>
-      </c>
-      <c r="D7">
+      <c r="G7">
+        <v>10</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7">
+        <v>5</v>
+      </c>
+      <c r="J7">
         <v>6</v>
-      </c>
-      <c r="E7">
-        <v>7</v>
-      </c>
-      <c r="F7">
-        <v>5</v>
-      </c>
-      <c r="G7">
-        <v>7</v>
-      </c>
-      <c r="H7">
-        <v>3</v>
-      </c>
-      <c r="I7">
-        <v>3</v>
-      </c>
-      <c r="J7">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -9749,7 +9726,7 @@
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -9804,113 +9781,89 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
       <c r="G2">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J3">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="J4">
+        <v>3</v>
+      </c>
+      <c r="E4">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J5">
+        <v>5</v>
+      </c>
+      <c r="B5">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C6">
-        <v>4</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>7</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C7">
-        <v>12</v>
-      </c>
-      <c r="D7">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E7">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="F7">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G7">
         <v>10</v>
@@ -9919,42 +9872,74 @@
         <v>6</v>
       </c>
       <c r="I7">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="J7">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>16</v>
+      </c>
+      <c r="D8">
+        <v>11</v>
+      </c>
+      <c r="E8">
+        <v>14</v>
+      </c>
+      <c r="F8">
+        <v>12</v>
+      </c>
+      <c r="G8">
+        <v>13</v>
+      </c>
+      <c r="H8">
+        <v>7</v>
+      </c>
+      <c r="I8">
+        <v>8</v>
+      </c>
+      <c r="J8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8">
-        <v>11</v>
-      </c>
-      <c r="C8">
+      <c r="B9">
         <v>18</v>
       </c>
-      <c r="D8">
+      <c r="C9">
+        <v>24</v>
+      </c>
+      <c r="D9">
+        <v>13</v>
+      </c>
+      <c r="E9">
         <v>20</v>
       </c>
-      <c r="E8">
+      <c r="F9">
+        <v>19</v>
+      </c>
+      <c r="G9">
+        <v>29</v>
+      </c>
+      <c r="H9">
         <v>18</v>
       </c>
-      <c r="F8">
-        <v>13</v>
-      </c>
-      <c r="G8">
+      <c r="I9">
         <v>15</v>
       </c>
-      <c r="H8">
-        <v>14</v>
-      </c>
-      <c r="I8">
-        <v>14</v>
-      </c>
-      <c r="J8">
-        <v>21</v>
+      <c r="J9">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -9964,13 +9949,13 @@
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" customWidth="1"/>
     <col min="3" max="3" width="4.7109375" customWidth="1"/>
     <col min="4" max="4" width="4.7109375" customWidth="1"/>
@@ -10018,10 +10003,10 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="E2">
         <v>1</v>
       </c>
       <c r="F2">
@@ -10029,9 +10014,6 @@
       </c>
       <c r="G2">
         <v>1</v>
-      </c>
-      <c r="I2">
-        <v>2</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -10041,113 +10023,115 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F3">
+      <c r="D3">
         <v>1</v>
       </c>
       <c r="G3">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>1</v>
-      </c>
-      <c r="C4">
-        <v>4</v>
-      </c>
-      <c r="D4">
-        <v>4</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
-      </c>
-      <c r="F4">
-        <v>5</v>
-      </c>
-      <c r="G4">
-        <v>3</v>
-      </c>
-      <c r="H4">
-        <v>10</v>
-      </c>
-      <c r="I4">
-        <v>6</v>
-      </c>
-      <c r="J4">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D5">
-        <v>11</v>
-      </c>
-      <c r="E5">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G5">
-        <v>6</v>
-      </c>
-      <c r="H5">
         <v>2</v>
       </c>
       <c r="I5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J5">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>6</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6">
-        <v>10</v>
-      </c>
-      <c r="C6">
-        <v>16</v>
-      </c>
-      <c r="D6">
-        <v>16</v>
-      </c>
-      <c r="E6">
-        <v>16</v>
-      </c>
-      <c r="F6">
-        <v>17</v>
-      </c>
-      <c r="G6">
-        <v>13</v>
-      </c>
-      <c r="H6">
-        <v>12</v>
-      </c>
-      <c r="I6">
-        <v>14</v>
-      </c>
-      <c r="J6">
-        <v>13</v>
+      <c r="B7">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>9</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>7</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>7</v>
+      </c>
+      <c r="H7">
+        <v>3</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+      <c r="J7">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -10384,13 +10368,13 @@
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" customWidth="1"/>
     <col min="3" max="3" width="4.7109375" customWidth="1"/>
     <col min="4" max="4" width="4.7109375" customWidth="1"/>
@@ -10441,16 +10425,16 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="F2">
+      <c r="D2">
         <v>1</v>
       </c>
       <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
         <v>2</v>
       </c>
     </row>
@@ -10458,110 +10442,138 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
         <v>1</v>
       </c>
       <c r="E3">
-        <v>4</v>
-      </c>
-      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="H3">
         <v>1</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J3">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4">
-        <v>9</v>
-      </c>
-      <c r="C4">
-        <v>4</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="J4">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>6</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5">
-        <v>6</v>
-      </c>
-      <c r="F5">
-        <v>6</v>
-      </c>
-      <c r="G5">
-        <v>2</v>
-      </c>
-      <c r="H5">
-        <v>5</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>7</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
         <v>10</v>
       </c>
-      <c r="B6">
-        <v>16</v>
-      </c>
-      <c r="C6">
-        <v>9</v>
-      </c>
-      <c r="D6">
-        <v>3</v>
-      </c>
-      <c r="E6">
+      <c r="C7">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>15</v>
+      </c>
+      <c r="F7">
+        <v>12</v>
+      </c>
+      <c r="G7">
+        <v>10</v>
+      </c>
+      <c r="H7">
+        <v>6</v>
+      </c>
+      <c r="I7">
+        <v>11</v>
+      </c>
+      <c r="J7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <v>18</v>
+      </c>
+      <c r="D8">
+        <v>20</v>
+      </c>
+      <c r="E8">
+        <v>18</v>
+      </c>
+      <c r="F8">
         <v>13</v>
       </c>
-      <c r="F6">
-        <v>10</v>
-      </c>
-      <c r="G6">
-        <v>4</v>
-      </c>
-      <c r="H6">
-        <v>8</v>
-      </c>
-      <c r="I6">
-        <v>6</v>
-      </c>
-      <c r="J6">
-        <v>6</v>
+      <c r="G8">
+        <v>15</v>
+      </c>
+      <c r="H8">
+        <v>14</v>
+      </c>
+      <c r="I8">
+        <v>14</v>
+      </c>
+      <c r="J8">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -10570,6 +10582,201 @@
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>12</v>
+      </c>
+      <c r="E6">
+        <v>9</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>8</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
+      <c r="J6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>17</v>
+      </c>
+      <c r="E7">
+        <v>12</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>12</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+      <c r="I7">
+        <v>7</v>
+      </c>
+      <c r="J7">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J5"/>
   <sheetViews>
@@ -10714,213 +10921,6 @@
       </c>
       <c r="J5">
         <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>2</v>
-      </c>
-      <c r="J3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>5</v>
-      </c>
-      <c r="E5">
-        <v>11</v>
-      </c>
-      <c r="F5">
-        <v>17</v>
-      </c>
-      <c r="G5">
-        <v>13</v>
-      </c>
-      <c r="H5">
-        <v>6</v>
-      </c>
-      <c r="I5">
-        <v>7</v>
-      </c>
-      <c r="J5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <v>12</v>
-      </c>
-      <c r="C6">
-        <v>7</v>
-      </c>
-      <c r="D6">
-        <v>13</v>
-      </c>
-      <c r="E6">
-        <v>14</v>
-      </c>
-      <c r="F6">
-        <v>25</v>
-      </c>
-      <c r="G6">
-        <v>8</v>
-      </c>
-      <c r="H6">
-        <v>6</v>
-      </c>
-      <c r="I6">
-        <v>3</v>
-      </c>
-      <c r="J6">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>18</v>
-      </c>
-      <c r="C7">
-        <v>13</v>
-      </c>
-      <c r="D7">
-        <v>20</v>
-      </c>
-      <c r="E7">
-        <v>26</v>
-      </c>
-      <c r="F7">
-        <v>44</v>
-      </c>
-      <c r="G7">
-        <v>22</v>
-      </c>
-      <c r="H7">
-        <v>15</v>
-      </c>
-      <c r="I7">
-        <v>13</v>
-      </c>
-      <c r="J7">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -10984,20 +10984,20 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E2">
-        <v>2</v>
+      <c r="C2">
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -11008,29 +11008,29 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="G3">
         <v>1</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
       <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
         <v>2</v>
       </c>
     </row>
@@ -11039,31 +11039,31 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F5">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="G5">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -11071,31 +11071,31 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>13</v>
+      </c>
+      <c r="E6">
+        <v>14</v>
+      </c>
+      <c r="F6">
+        <v>25</v>
+      </c>
+      <c r="G6">
+        <v>8</v>
+      </c>
+      <c r="H6">
+        <v>6</v>
+      </c>
+      <c r="I6">
+        <v>3</v>
+      </c>
+      <c r="J6">
         <v>12</v>
-      </c>
-      <c r="D6">
-        <v>18</v>
-      </c>
-      <c r="E6">
-        <v>19</v>
-      </c>
-      <c r="F6">
-        <v>21</v>
-      </c>
-      <c r="G6">
-        <v>11</v>
-      </c>
-      <c r="H6">
-        <v>2</v>
-      </c>
-      <c r="I6">
-        <v>4</v>
-      </c>
-      <c r="J6">
-        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -11103,31 +11103,31 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C7">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D7">
         <v>20</v>
       </c>
       <c r="E7">
+        <v>26</v>
+      </c>
+      <c r="F7">
+        <v>44</v>
+      </c>
+      <c r="G7">
         <v>22</v>
       </c>
-      <c r="F7">
-        <v>27</v>
-      </c>
-      <c r="G7">
+      <c r="H7">
+        <v>15</v>
+      </c>
+      <c r="I7">
         <v>13</v>
       </c>
-      <c r="H7">
-        <v>8</v>
-      </c>
-      <c r="I7">
-        <v>14</v>
-      </c>
       <c r="J7">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2023-08-04
</commit_message>
<xml_diff>
--- a/output/cta-index-crime-ytd.xlsx
+++ b/output/cta-index-crime-ytd.xlsx
@@ -30,26 +30,26 @@
     <sheet name="Ashburn" sheetId="21" r:id="rId21"/>
     <sheet name="New City" sheetId="22" r:id="rId22"/>
     <sheet name="Lower West Side" sheetId="23" r:id="rId23"/>
-    <sheet name="Irving Park" sheetId="24" r:id="rId24"/>
-    <sheet name="Rogers Park" sheetId="25" r:id="rId25"/>
-    <sheet name="Kenwood" sheetId="26" r:id="rId26"/>
-    <sheet name="Roseland" sheetId="27" r:id="rId27"/>
-    <sheet name="Austin" sheetId="28" r:id="rId28"/>
-    <sheet name="Hyde Park" sheetId="29" r:id="rId29"/>
-    <sheet name="River North" sheetId="30" r:id="rId30"/>
-    <sheet name="Fuller Park" sheetId="31" r:id="rId31"/>
-    <sheet name="Old Town" sheetId="32" r:id="rId32"/>
-    <sheet name="Printers Row" sheetId="33" r:id="rId33"/>
-    <sheet name="Lincoln Park" sheetId="34" r:id="rId34"/>
-    <sheet name="Chicago Lawn" sheetId="35" r:id="rId35"/>
-    <sheet name="Uptown" sheetId="36" r:id="rId36"/>
-    <sheet name="Wrigleyville" sheetId="37" r:id="rId37"/>
-    <sheet name="Logan Square" sheetId="38" r:id="rId38"/>
-    <sheet name="Edgewater" sheetId="39" r:id="rId39"/>
-    <sheet name="South Chicago" sheetId="40" r:id="rId40"/>
-    <sheet name="West Elsdon" sheetId="41" r:id="rId41"/>
-    <sheet name="Little Italy, UIC" sheetId="42" r:id="rId42"/>
-    <sheet name="Sheffield &amp; DePaul" sheetId="43" r:id="rId43"/>
+    <sheet name="South Chicago" sheetId="24" r:id="rId24"/>
+    <sheet name="Lincoln Park" sheetId="25" r:id="rId25"/>
+    <sheet name="Sheffield &amp; DePaul" sheetId="26" r:id="rId26"/>
+    <sheet name="Rogers Park" sheetId="27" r:id="rId27"/>
+    <sheet name="Edgewater" sheetId="28" r:id="rId28"/>
+    <sheet name="Kenwood" sheetId="29" r:id="rId29"/>
+    <sheet name="Roseland" sheetId="30" r:id="rId30"/>
+    <sheet name="Austin" sheetId="31" r:id="rId31"/>
+    <sheet name="Hyde Park" sheetId="32" r:id="rId32"/>
+    <sheet name="River North" sheetId="33" r:id="rId33"/>
+    <sheet name="Fuller Park" sheetId="34" r:id="rId34"/>
+    <sheet name="Old Town" sheetId="35" r:id="rId35"/>
+    <sheet name="Printers Row" sheetId="36" r:id="rId36"/>
+    <sheet name="Chicago Lawn" sheetId="37" r:id="rId37"/>
+    <sheet name="Uptown" sheetId="38" r:id="rId38"/>
+    <sheet name="Wrigleyville" sheetId="39" r:id="rId39"/>
+    <sheet name="Logan Square" sheetId="40" r:id="rId40"/>
+    <sheet name="Irving Park" sheetId="41" r:id="rId41"/>
+    <sheet name="West Elsdon" sheetId="42" r:id="rId42"/>
+    <sheet name="Little Italy, UIC" sheetId="43" r:id="rId43"/>
     <sheet name="Bucktown" sheetId="44" r:id="rId44"/>
     <sheet name="Woodlawn" sheetId="45" r:id="rId45"/>
     <sheet name="Bridgeport" sheetId="46" r:id="rId46"/>
@@ -6749,6 +6749,196 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
+      <c r="F5">
+        <v>6</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>13</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6">
+        <v>8</v>
+      </c>
+      <c r="I6">
+        <v>6</v>
+      </c>
+      <c r="J6">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -6803,13 +6993,7 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="I2">
+      <c r="D2">
         <v>1</v>
       </c>
       <c r="J2">
@@ -6820,27 +7004,21 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
+      <c r="F3">
         <v>1</v>
       </c>
       <c r="G3">
-        <v>2</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4">
+      <c r="B4">
         <v>1</v>
       </c>
     </row>
@@ -6848,29 +7026,26 @@
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
       <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
         <v>2</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I5">
         <v>1</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -6878,25 +7053,22 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D6">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E6">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F6">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G6">
-        <v>8</v>
-      </c>
-      <c r="H6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I6">
         <v>4</v>
@@ -6910,252 +7082,31 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C7">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D7">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E7">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F7">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="G7">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I7">
+        <v>5</v>
+      </c>
+      <c r="J7">
         <v>7</v>
-      </c>
-      <c r="J7">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>7</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>4</v>
-      </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>7</v>
-      </c>
-      <c r="D6">
-        <v>7</v>
-      </c>
-      <c r="E6">
-        <v>3</v>
-      </c>
-      <c r="F6">
-        <v>10</v>
-      </c>
-      <c r="G6">
-        <v>4</v>
-      </c>
-      <c r="H6">
-        <v>9</v>
-      </c>
-      <c r="I6">
-        <v>10</v>
-      </c>
-      <c r="J6">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>26</v>
-      </c>
-      <c r="C7">
-        <v>38</v>
-      </c>
-      <c r="D7">
-        <v>26</v>
-      </c>
-      <c r="E7">
-        <v>43</v>
-      </c>
-      <c r="F7">
-        <v>19</v>
-      </c>
-      <c r="G7">
-        <v>19</v>
-      </c>
-      <c r="H7">
-        <v>17</v>
-      </c>
-      <c r="I7">
-        <v>16</v>
-      </c>
-      <c r="J7">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8">
-        <v>28</v>
-      </c>
-      <c r="C8">
-        <v>48</v>
-      </c>
-      <c r="D8">
-        <v>35</v>
-      </c>
-      <c r="E8">
-        <v>54</v>
-      </c>
-      <c r="F8">
-        <v>31</v>
-      </c>
-      <c r="G8">
-        <v>28</v>
-      </c>
-      <c r="H8">
-        <v>29</v>
-      </c>
-      <c r="I8">
-        <v>29</v>
-      </c>
-      <c r="J8">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -7219,15 +7170,42 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
       <c r="H2">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G3">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
         <v>1</v>
       </c>
     </row>
@@ -7235,15 +7213,42 @@
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
       <c r="I4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
       <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>6</v>
+      </c>
+      <c r="J5">
         <v>1</v>
       </c>
     </row>
@@ -7252,25 +7257,31 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E6">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="F6">
-        <v>3</v>
+        <v>21</v>
+      </c>
+      <c r="G6">
+        <v>11</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
       </c>
       <c r="J6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -7278,31 +7289,31 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E7">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="F7">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="G7">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="H7">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="J7">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -7311,252 +7322,6 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
-      <c r="H2">
-        <v>2</v>
-      </c>
-      <c r="I2">
-        <v>5</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>4</v>
-      </c>
-      <c r="F3">
-        <v>4</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>4</v>
-      </c>
-      <c r="I3">
-        <v>6</v>
-      </c>
-      <c r="J3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>12</v>
-      </c>
-      <c r="C8">
-        <v>11</v>
-      </c>
-      <c r="D8">
-        <v>3</v>
-      </c>
-      <c r="E8">
-        <v>10</v>
-      </c>
-      <c r="F8">
-        <v>4</v>
-      </c>
-      <c r="G8">
-        <v>9</v>
-      </c>
-      <c r="H8">
-        <v>10</v>
-      </c>
-      <c r="I8">
-        <v>16</v>
-      </c>
-      <c r="J8">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>28</v>
-      </c>
-      <c r="C9">
-        <v>28</v>
-      </c>
-      <c r="D9">
-        <v>25</v>
-      </c>
-      <c r="E9">
-        <v>28</v>
-      </c>
-      <c r="F9">
-        <v>27</v>
-      </c>
-      <c r="G9">
-        <v>18</v>
-      </c>
-      <c r="H9">
-        <v>18</v>
-      </c>
-      <c r="I9">
-        <v>23</v>
-      </c>
-      <c r="J9">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10">
-        <v>42</v>
-      </c>
-      <c r="C10">
-        <v>44</v>
-      </c>
-      <c r="D10">
-        <v>32</v>
-      </c>
-      <c r="E10">
-        <v>45</v>
-      </c>
-      <c r="F10">
-        <v>37</v>
-      </c>
-      <c r="G10">
-        <v>30</v>
-      </c>
-      <c r="H10">
-        <v>34</v>
-      </c>
-      <c r="I10">
-        <v>51</v>
-      </c>
-      <c r="J10">
-        <v>43</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J8"/>
   <sheetViews>
@@ -7612,89 +7377,68 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>4</v>
-      </c>
       <c r="C2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="H2">
-        <v>2</v>
-      </c>
       <c r="I2">
-        <v>3</v>
-      </c>
-      <c r="J2">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
       <c r="C3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <v>4</v>
       </c>
       <c r="H3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J3">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="H4">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>2</v>
+        <v>7</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -7702,31 +7446,31 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C6">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D6">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E6">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="F6">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G6">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="H6">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="I6">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J6">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -7734,31 +7478,31 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D7">
+        <v>26</v>
+      </c>
+      <c r="E7">
+        <v>43</v>
+      </c>
+      <c r="F7">
+        <v>19</v>
+      </c>
+      <c r="G7">
+        <v>19</v>
+      </c>
+      <c r="H7">
         <v>17</v>
       </c>
-      <c r="E7">
-        <v>34</v>
-      </c>
-      <c r="F7">
-        <v>51</v>
-      </c>
-      <c r="G7">
-        <v>49</v>
-      </c>
-      <c r="H7">
-        <v>18</v>
-      </c>
       <c r="I7">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="J7">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -7766,31 +7510,31 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="C8">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="D8">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E8">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="F8">
-        <v>84</v>
+        <v>31</v>
       </c>
       <c r="G8">
-        <v>70</v>
+        <v>28</v>
       </c>
       <c r="H8">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="I8">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="J8">
-        <v>42</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -7798,7 +7542,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -7854,7 +7598,22 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
       <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2">
         <v>1</v>
       </c>
     </row>
@@ -7862,17 +7621,17 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -7880,25 +7639,31 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J4">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -7906,31 +7671,31 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E5">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F5">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J5">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -7938,31 +7703,178 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="E6">
+        <v>16</v>
+      </c>
+      <c r="F6">
+        <v>17</v>
+      </c>
+      <c r="G6">
+        <v>13</v>
+      </c>
+      <c r="H6">
+        <v>12</v>
+      </c>
+      <c r="I6">
+        <v>14</v>
+      </c>
+      <c r="J6">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
       <c r="F6">
-        <v>4</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H6">
-        <v>5</v>
-      </c>
-      <c r="I6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -8165,6 +8077,666 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <v>6</v>
+      </c>
+      <c r="J3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>11</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>10</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+      <c r="G8">
+        <v>9</v>
+      </c>
+      <c r="H8">
+        <v>10</v>
+      </c>
+      <c r="I8">
+        <v>16</v>
+      </c>
+      <c r="J8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>28</v>
+      </c>
+      <c r="C9">
+        <v>28</v>
+      </c>
+      <c r="D9">
+        <v>25</v>
+      </c>
+      <c r="E9">
+        <v>28</v>
+      </c>
+      <c r="F9">
+        <v>27</v>
+      </c>
+      <c r="G9">
+        <v>18</v>
+      </c>
+      <c r="H9">
+        <v>18</v>
+      </c>
+      <c r="I9">
+        <v>23</v>
+      </c>
+      <c r="J9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>42</v>
+      </c>
+      <c r="C10">
+        <v>44</v>
+      </c>
+      <c r="D10">
+        <v>32</v>
+      </c>
+      <c r="E10">
+        <v>45</v>
+      </c>
+      <c r="F10">
+        <v>37</v>
+      </c>
+      <c r="G10">
+        <v>30</v>
+      </c>
+      <c r="H10">
+        <v>34</v>
+      </c>
+      <c r="I10">
+        <v>51</v>
+      </c>
+      <c r="J10">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>6</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+      <c r="J2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>22</v>
+      </c>
+      <c r="D6">
+        <v>14</v>
+      </c>
+      <c r="E6">
+        <v>18</v>
+      </c>
+      <c r="F6">
+        <v>22</v>
+      </c>
+      <c r="G6">
+        <v>16</v>
+      </c>
+      <c r="H6">
+        <v>19</v>
+      </c>
+      <c r="I6">
+        <v>13</v>
+      </c>
+      <c r="J6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>27</v>
+      </c>
+      <c r="C7">
+        <v>32</v>
+      </c>
+      <c r="D7">
+        <v>17</v>
+      </c>
+      <c r="E7">
+        <v>34</v>
+      </c>
+      <c r="F7">
+        <v>51</v>
+      </c>
+      <c r="G7">
+        <v>49</v>
+      </c>
+      <c r="H7">
+        <v>18</v>
+      </c>
+      <c r="I7">
+        <v>24</v>
+      </c>
+      <c r="J7">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>49</v>
+      </c>
+      <c r="C8">
+        <v>62</v>
+      </c>
+      <c r="D8">
+        <v>39</v>
+      </c>
+      <c r="E8">
+        <v>60</v>
+      </c>
+      <c r="F8">
+        <v>84</v>
+      </c>
+      <c r="G8">
+        <v>70</v>
+      </c>
+      <c r="H8">
+        <v>42</v>
+      </c>
+      <c r="I8">
+        <v>44</v>
+      </c>
+      <c r="J8">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>9</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="J6">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -8367,7 +8939,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J9"/>
   <sheetViews>
@@ -8584,7 +9156,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J7"/>
   <sheetViews>
@@ -8788,7 +9360,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -8950,601 +9522,6 @@
       </c>
       <c r="J6">
         <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>4</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <v>7</v>
-      </c>
-      <c r="D6">
-        <v>10</v>
-      </c>
-      <c r="E6">
-        <v>3</v>
-      </c>
-      <c r="F6">
-        <v>10</v>
-      </c>
-      <c r="G6">
-        <v>4</v>
-      </c>
-      <c r="I6">
-        <v>4</v>
-      </c>
-      <c r="J6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>10</v>
-      </c>
-      <c r="C7">
-        <v>8</v>
-      </c>
-      <c r="D7">
-        <v>11</v>
-      </c>
-      <c r="E7">
-        <v>7</v>
-      </c>
-      <c r="F7">
-        <v>13</v>
-      </c>
-      <c r="G7">
-        <v>5</v>
-      </c>
-      <c r="H7">
-        <v>3</v>
-      </c>
-      <c r="I7">
-        <v>5</v>
-      </c>
-      <c r="J7">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>3</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>2</v>
-      </c>
-      <c r="J3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>7</v>
-      </c>
-      <c r="D5">
-        <v>6</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>3</v>
-      </c>
-      <c r="G5">
-        <v>3</v>
-      </c>
-      <c r="H5">
-        <v>3</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <v>11</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6">
-        <v>3</v>
-      </c>
-      <c r="F6">
-        <v>5</v>
-      </c>
-      <c r="G6">
-        <v>4</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6">
-        <v>3</v>
-      </c>
-      <c r="J6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>17</v>
-      </c>
-      <c r="C7">
-        <v>12</v>
-      </c>
-      <c r="D7">
-        <v>12</v>
-      </c>
-      <c r="E7">
-        <v>5</v>
-      </c>
-      <c r="F7">
-        <v>9</v>
-      </c>
-      <c r="G7">
-        <v>10</v>
-      </c>
-      <c r="H7">
-        <v>5</v>
-      </c>
-      <c r="I7">
-        <v>5</v>
-      </c>
-      <c r="J7">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
-      <c r="H2">
-        <v>5</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
-      <c r="G3">
-        <v>4</v>
-      </c>
-      <c r="I3">
-        <v>2</v>
-      </c>
-      <c r="J3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>5</v>
-      </c>
-      <c r="C7">
-        <v>5</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>4</v>
-      </c>
-      <c r="G7">
-        <v>11</v>
-      </c>
-      <c r="H7">
-        <v>6</v>
-      </c>
-      <c r="I7">
-        <v>4</v>
-      </c>
-      <c r="J7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <v>12</v>
-      </c>
-      <c r="C8">
-        <v>16</v>
-      </c>
-      <c r="D8">
-        <v>11</v>
-      </c>
-      <c r="E8">
-        <v>14</v>
-      </c>
-      <c r="F8">
-        <v>12</v>
-      </c>
-      <c r="G8">
-        <v>13</v>
-      </c>
-      <c r="H8">
-        <v>7</v>
-      </c>
-      <c r="I8">
-        <v>8</v>
-      </c>
-      <c r="J8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>18</v>
-      </c>
-      <c r="C9">
-        <v>24</v>
-      </c>
-      <c r="D9">
-        <v>13</v>
-      </c>
-      <c r="E9">
-        <v>20</v>
-      </c>
-      <c r="F9">
-        <v>19</v>
-      </c>
-      <c r="G9">
-        <v>30</v>
-      </c>
-      <c r="H9">
-        <v>18</v>
-      </c>
-      <c r="I9">
-        <v>15</v>
-      </c>
-      <c r="J9">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -9608,19 +9585,13 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
+      <c r="D2">
         <v>1</v>
       </c>
       <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="J2">
+        <v>3</v>
+      </c>
+      <c r="H2">
         <v>1</v>
       </c>
     </row>
@@ -9628,20 +9599,26 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
         <v>1</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -9656,20 +9633,23 @@
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5">
-        <v>2</v>
+      <c r="B5">
+        <v>7</v>
       </c>
       <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5">
         <v>1</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G5">
-        <v>2</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -9680,31 +9660,31 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C6">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D6">
         <v>4</v>
       </c>
       <c r="E6">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F6">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -9712,31 +9692,31 @@
         <v>10</v>
       </c>
       <c r="B7">
+        <v>17</v>
+      </c>
+      <c r="C7">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>12</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
         <v>9</v>
       </c>
-      <c r="C7">
-        <v>9</v>
-      </c>
-      <c r="D7">
-        <v>6</v>
-      </c>
-      <c r="E7">
-        <v>7</v>
-      </c>
-      <c r="F7">
-        <v>5</v>
-      </c>
       <c r="G7">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J7">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -9746,7 +9726,7 @@
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -9801,157 +9781,165 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
       <c r="G2">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J3">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="J4">
+        <v>3</v>
+      </c>
+      <c r="E4">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J5">
+        <v>5</v>
+      </c>
+      <c r="B5">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C6">
-        <v>4</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>7</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C7">
-        <v>12</v>
-      </c>
-      <c r="D7">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E7">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="F7">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H7">
         <v>6</v>
       </c>
       <c r="I7">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="J7">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>16</v>
+      </c>
+      <c r="D8">
+        <v>11</v>
+      </c>
+      <c r="E8">
+        <v>14</v>
+      </c>
+      <c r="F8">
+        <v>12</v>
+      </c>
+      <c r="G8">
+        <v>13</v>
+      </c>
+      <c r="H8">
+        <v>7</v>
+      </c>
+      <c r="I8">
+        <v>8</v>
+      </c>
+      <c r="J8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8">
-        <v>11</v>
-      </c>
-      <c r="C8">
+      <c r="B9">
         <v>18</v>
       </c>
-      <c r="D8">
+      <c r="C9">
+        <v>24</v>
+      </c>
+      <c r="D9">
+        <v>13</v>
+      </c>
+      <c r="E9">
         <v>20</v>
       </c>
-      <c r="E8">
+      <c r="F9">
+        <v>19</v>
+      </c>
+      <c r="G9">
+        <v>30</v>
+      </c>
+      <c r="H9">
         <v>18</v>
       </c>
-      <c r="F8">
-        <v>13</v>
-      </c>
-      <c r="G8">
+      <c r="I9">
         <v>15</v>
       </c>
-      <c r="H8">
-        <v>14</v>
-      </c>
-      <c r="I8">
-        <v>15</v>
-      </c>
-      <c r="J8">
-        <v>21</v>
+      <c r="J9">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -9961,13 +9949,13 @@
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" customWidth="1"/>
     <col min="3" max="3" width="4.7109375" customWidth="1"/>
     <col min="4" max="4" width="4.7109375" customWidth="1"/>
@@ -10015,10 +10003,10 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="E2">
         <v>1</v>
       </c>
       <c r="F2">
@@ -10026,9 +10014,6 @@
       </c>
       <c r="G2">
         <v>1</v>
-      </c>
-      <c r="I2">
-        <v>2</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -10038,113 +10023,115 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F3">
+      <c r="D3">
         <v>1</v>
       </c>
       <c r="G3">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>1</v>
-      </c>
-      <c r="C4">
-        <v>4</v>
-      </c>
-      <c r="D4">
-        <v>4</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
-      </c>
-      <c r="F4">
-        <v>5</v>
-      </c>
-      <c r="G4">
-        <v>3</v>
-      </c>
-      <c r="H4">
-        <v>10</v>
-      </c>
-      <c r="I4">
-        <v>6</v>
-      </c>
-      <c r="J4">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D5">
-        <v>11</v>
-      </c>
-      <c r="E5">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G5">
-        <v>6</v>
-      </c>
-      <c r="H5">
         <v>2</v>
       </c>
       <c r="I5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J5">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>6</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6">
-        <v>11</v>
-      </c>
-      <c r="C6">
-        <v>16</v>
-      </c>
-      <c r="D6">
-        <v>16</v>
-      </c>
-      <c r="E6">
-        <v>16</v>
-      </c>
-      <c r="F6">
-        <v>17</v>
-      </c>
-      <c r="G6">
-        <v>13</v>
-      </c>
-      <c r="H6">
-        <v>12</v>
-      </c>
-      <c r="I6">
-        <v>14</v>
-      </c>
-      <c r="J6">
-        <v>13</v>
+      <c r="B7">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>9</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>7</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>7</v>
+      </c>
+      <c r="H7">
+        <v>3</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+      <c r="J7">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -10381,13 +10368,13 @@
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" customWidth="1"/>
     <col min="3" max="3" width="4.7109375" customWidth="1"/>
     <col min="4" max="4" width="4.7109375" customWidth="1"/>
@@ -10438,16 +10425,16 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="F2">
+      <c r="D2">
         <v>1</v>
       </c>
       <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
         <v>2</v>
       </c>
     </row>
@@ -10455,113 +10442,138 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
         <v>1</v>
       </c>
       <c r="E3">
-        <v>4</v>
-      </c>
-      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="H3">
         <v>1</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J3">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4">
-        <v>9</v>
-      </c>
-      <c r="C4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
+      <c r="J4">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>6</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5">
-        <v>6</v>
-      </c>
-      <c r="F5">
-        <v>6</v>
-      </c>
-      <c r="G5">
-        <v>2</v>
-      </c>
-      <c r="H5">
-        <v>5</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>7</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
         <v>10</v>
       </c>
-      <c r="B6">
-        <v>16</v>
-      </c>
-      <c r="C6">
-        <v>9</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6">
+      <c r="C7">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>15</v>
+      </c>
+      <c r="F7">
+        <v>12</v>
+      </c>
+      <c r="G7">
+        <v>10</v>
+      </c>
+      <c r="H7">
+        <v>6</v>
+      </c>
+      <c r="I7">
+        <v>12</v>
+      </c>
+      <c r="J7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <v>18</v>
+      </c>
+      <c r="D8">
+        <v>20</v>
+      </c>
+      <c r="E8">
+        <v>18</v>
+      </c>
+      <c r="F8">
         <v>13</v>
       </c>
-      <c r="F6">
-        <v>10</v>
-      </c>
-      <c r="G6">
-        <v>4</v>
-      </c>
-      <c r="H6">
-        <v>8</v>
-      </c>
-      <c r="I6">
-        <v>6</v>
-      </c>
-      <c r="J6">
-        <v>6</v>
+      <c r="G8">
+        <v>15</v>
+      </c>
+      <c r="H8">
+        <v>14</v>
+      </c>
+      <c r="I8">
+        <v>15</v>
+      </c>
+      <c r="J8">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -10570,6 +10582,201 @@
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>12</v>
+      </c>
+      <c r="E6">
+        <v>9</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>8</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
+      <c r="J6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>17</v>
+      </c>
+      <c r="E7">
+        <v>12</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>12</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+      <c r="I7">
+        <v>7</v>
+      </c>
+      <c r="J7">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J5"/>
   <sheetViews>
@@ -10714,213 +10921,6 @@
       </c>
       <c r="J5">
         <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>2</v>
-      </c>
-      <c r="J3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>5</v>
-      </c>
-      <c r="E5">
-        <v>11</v>
-      </c>
-      <c r="F5">
-        <v>17</v>
-      </c>
-      <c r="G5">
-        <v>13</v>
-      </c>
-      <c r="H5">
-        <v>6</v>
-      </c>
-      <c r="I5">
-        <v>7</v>
-      </c>
-      <c r="J5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <v>12</v>
-      </c>
-      <c r="C6">
-        <v>7</v>
-      </c>
-      <c r="D6">
-        <v>13</v>
-      </c>
-      <c r="E6">
-        <v>14</v>
-      </c>
-      <c r="F6">
-        <v>25</v>
-      </c>
-      <c r="G6">
-        <v>8</v>
-      </c>
-      <c r="H6">
-        <v>6</v>
-      </c>
-      <c r="I6">
-        <v>3</v>
-      </c>
-      <c r="J6">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>18</v>
-      </c>
-      <c r="C7">
-        <v>13</v>
-      </c>
-      <c r="D7">
-        <v>20</v>
-      </c>
-      <c r="E7">
-        <v>26</v>
-      </c>
-      <c r="F7">
-        <v>44</v>
-      </c>
-      <c r="G7">
-        <v>22</v>
-      </c>
-      <c r="H7">
-        <v>15</v>
-      </c>
-      <c r="I7">
-        <v>13</v>
-      </c>
-      <c r="J7">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -10984,20 +10984,20 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E2">
-        <v>2</v>
+      <c r="C2">
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -11008,29 +11008,29 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="G3">
         <v>1</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
       <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
         <v>2</v>
       </c>
     </row>
@@ -11039,31 +11039,31 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F5">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="G5">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -11071,31 +11071,31 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>13</v>
+      </c>
+      <c r="E6">
+        <v>14</v>
+      </c>
+      <c r="F6">
+        <v>25</v>
+      </c>
+      <c r="G6">
+        <v>8</v>
+      </c>
+      <c r="H6">
+        <v>6</v>
+      </c>
+      <c r="I6">
+        <v>3</v>
+      </c>
+      <c r="J6">
         <v>12</v>
-      </c>
-      <c r="D6">
-        <v>18</v>
-      </c>
-      <c r="E6">
-        <v>20</v>
-      </c>
-      <c r="F6">
-        <v>21</v>
-      </c>
-      <c r="G6">
-        <v>11</v>
-      </c>
-      <c r="H6">
-        <v>2</v>
-      </c>
-      <c r="I6">
-        <v>4</v>
-      </c>
-      <c r="J6">
-        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -11103,31 +11103,31 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C7">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D7">
         <v>20</v>
       </c>
       <c r="E7">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F7">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="G7">
+        <v>22</v>
+      </c>
+      <c r="H7">
+        <v>15</v>
+      </c>
+      <c r="I7">
         <v>13</v>
       </c>
-      <c r="H7">
-        <v>8</v>
-      </c>
-      <c r="I7">
-        <v>14</v>
-      </c>
       <c r="J7">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>